<commit_message>
ajout fonction polynomiale de 2e degré
</commit_message>
<xml_diff>
--- a/EE03.xlsx
+++ b/EE03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olimo\remise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A7D284-8E3A-46AE-A06F-C42E4781CEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1239C6B0-CF15-4812-88FB-95538D988EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CC6D29E-86BE-4D22-95F8-090C74A419FC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Fonctions mathématiques</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>P 2e degré</t>
   </si>
 </sst>
 </file>
@@ -271,18 +274,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -290,25 +284,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -318,6 +299,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -374,7 +382,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1023,7 +1031,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1660,6 +1668,655 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-EE79-46B1-9D9C-84B3CCA1D900}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>p2e</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$M$14:$M$114</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-9.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-8.0000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-7.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-7.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-7.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-6.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-6.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-6.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-5.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-5.6000000000000201</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-5.4000000000000199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-5.2000000000000197</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-5.0000000000000204</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-4.8000000000000203</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.6000000000000201</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-4.4000000000000199</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-4.2000000000000197</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-4.0000000000000204</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.8000000000000198</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-3.6000000000000201</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-3.4000000000000199</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-3.2000000000000202</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-3.00000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-2.80000000000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-2.6000000000000298</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-2.4000000000000301</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-2.2000000000000299</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.0000000000000302</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.80000000000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.6000000000000301</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.4000000000000301</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.2000000000000299</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1.00000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.80000000000002902</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.60000000000002995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.400000000000031</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.20000000000002899</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-4.0856207306205799E-14</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.19999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.80000000000000104</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>7.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>7.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8.3999999999999009</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>8.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8.7999999999998995</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>8.9999999999999005</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.3999999999999009</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.7999999999998995</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>9.9999999999999005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$P$14:$P$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.440000000000026</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.560000000000016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69.239999999999981</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.840000000000011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.759999999999991</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.76000000000014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>53.840000000000146</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.000000000000149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.240000000000137</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45.56000000000013</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42.960000000000129</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>40.440000000000126</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38.000000000000114</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>35.640000000000114</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.360000000000113</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31.16000000000011</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29.040000000000106</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27.000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25.040000000000095</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.160000000000181</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.360000000000174</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19.640000000000164</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>18.000000000000163</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16.440000000000154</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.960000000000145</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13.560000000000134</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.240000000000125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.000000000000123</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.84000000000011</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.7600000000001046</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.7600000000000957</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.8400000000000896</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.0000000000000808</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.2400000000001077</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.5600000000000955</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.9600000000000843</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.4400000000000714</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.0000000000000604</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.6400000000000481</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2.3600000000000363</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.1600000000000241</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.040000000000012</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.0399999999999885</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.1599999999999762</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.359999999999963</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.6399999999999535</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.9999999999999183</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.4399999999999977</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.5600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.2400000000000038</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.84</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7.76</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8.7600000000000016</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>9.84</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12.240000000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>13.559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>14.96</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>16.439999999999998</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>19.64</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>21.36</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>23.16</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>25.04</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>29.039999999998958</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>31.159999999998917</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>33.359999999998877</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>35.639999999998842</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>37.999999999998799</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>40.439999999998761</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>42.959999999998722</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>45.559999999998681</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>48.239999999998645</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>50.999999999998593</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>53.839999999998554</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>56.75999999999852</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>59.759999999998485</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>62.839999999998447</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>65.999999999998394</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>69.239999999998361</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>72.559999999998325</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>75.959999999998288</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>79.43999999999825</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>82.999999999998195</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>86.639999999998167</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>90.359999999998138</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>94.159999999998092</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>98.039999999998031</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>101.99999999999801</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>106.03999999999795</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>110.15999999999794</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>114.35999999999788</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>118.63999999999783</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>122.99999999999781</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4311-4F93-9787-68D128188BEB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2748,190 +3405,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230CD6A0-05B3-4CAD-B94C-3912BC4D5061}">
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:15" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:16" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8">
+      <c r="E6" s="19"/>
+      <c r="F6" s="4">
         <v>3</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="4">
         <v>2</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="4">
         <v>3</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="4">
         <v>4</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10">
+      <c r="E7" s="20"/>
+      <c r="F7" s="5">
         <v>1</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="5">
         <v>2</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12">
+      <c r="E8" s="21"/>
+      <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="6">
         <v>2</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="6">
         <v>3</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15">
+      <c r="E9" s="16"/>
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="7">
         <v>3</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="7">
         <v>4</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17">
+      <c r="E10" s="17"/>
+      <c r="F10" s="8">
         <v>1</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="8">
         <v>2</v>
       </c>
-      <c r="H10" s="17">
+      <c r="H10" s="8">
         <v>3</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="8">
         <v>4</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="8">
         <v>5</v>
       </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>7</v>
       </c>
@@ -2940,1370 +3597,1779 @@
         <v>10</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="19">
+      <c r="F11" s="9">
         <v>1</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="9">
         <v>2</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="9">
         <v>3</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="9">
         <v>4</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M12" s="25" t="s">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="N12" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O12" s="22" t="s">
+      <c r="O12" s="15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M13" s="25"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="22"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M14" s="24">
+      <c r="P12" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M13" s="13"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="25"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M14" s="12">
         <v>-10</v>
       </c>
-      <c r="N14" s="21">
+      <c r="N14" s="10">
         <f>$F$6*ABS($G$6*M14+$H$6)+$I$6</f>
         <v>55</v>
       </c>
-      <c r="O14" s="23">
+      <c r="O14" s="11">
         <f>$F$7*M14+G7</f>
         <v>-8</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M15" s="24">
+      <c r="P14" s="26">
+        <f>$F$8*(M14^2)+$G$8*M14+$H$8</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M15" s="12">
         <v>-9.8000000000000007</v>
       </c>
-      <c r="N15" s="21">
+      <c r="N15" s="10">
         <f t="shared" ref="N15:N78" si="0">$F$6*ABS($G$6*M15+$H$6)+$I$6</f>
         <v>53.800000000000004</v>
       </c>
-      <c r="O15" s="23">
+      <c r="O15" s="11">
         <f t="shared" ref="O15:O78" si="1">$F$7*M15+G8</f>
         <v>-7.8000000000000007</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M16" s="24">
+      <c r="P15" s="26">
+        <f t="shared" ref="P15:P78" si="2">$F$8*(M15^2)+$G$8*M15+$H$8</f>
+        <v>79.440000000000026</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M16" s="12">
         <v>-9.6</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16" s="10">
         <f t="shared" si="0"/>
         <v>52.599999999999994</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="11">
         <f t="shared" si="1"/>
         <v>-7.6</v>
       </c>
-    </row>
-    <row r="17" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M17" s="24">
+      <c r="P16" s="26">
+        <f t="shared" si="2"/>
+        <v>75.959999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M17" s="12">
         <v>-9.4</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="10">
         <f t="shared" si="0"/>
         <v>51.400000000000006</v>
       </c>
-      <c r="O17" s="23">
+      <c r="O17" s="11">
         <f t="shared" si="1"/>
         <v>-7.4</v>
       </c>
-    </row>
-    <row r="18" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M18" s="24">
+      <c r="P17" s="26">
+        <f t="shared" si="2"/>
+        <v>72.560000000000016</v>
+      </c>
+    </row>
+    <row r="18" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M18" s="12">
         <v>-9.1999999999999993</v>
       </c>
-      <c r="N18" s="21">
+      <c r="N18" s="10">
         <f t="shared" si="0"/>
         <v>50.199999999999996</v>
       </c>
-      <c r="O18" s="23">
+      <c r="O18" s="11">
         <f t="shared" si="1"/>
         <v>-7.1999999999999993</v>
       </c>
-    </row>
-    <row r="19" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M19" s="24">
+      <c r="P18" s="26">
+        <f t="shared" si="2"/>
+        <v>69.239999999999981</v>
+      </c>
+    </row>
+    <row r="19" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M19" s="12">
         <v>-9</v>
       </c>
-      <c r="N19" s="21">
+      <c r="N19" s="10">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="O19" s="23">
+      <c r="O19" s="11">
         <f t="shared" si="1"/>
         <v>-9</v>
       </c>
-    </row>
-    <row r="20" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M20" s="24">
+      <c r="P19" s="26">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M20" s="12">
         <v>-8.8000000000000007</v>
       </c>
-      <c r="N20" s="21">
+      <c r="N20" s="10">
         <f t="shared" si="0"/>
         <v>47.800000000000004</v>
       </c>
-      <c r="O20" s="23">
+      <c r="O20" s="11">
         <f t="shared" si="1"/>
         <v>-8.8000000000000007</v>
       </c>
-    </row>
-    <row r="21" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M21" s="24">
+      <c r="P20" s="26">
+        <f t="shared" si="2"/>
+        <v>62.840000000000011</v>
+      </c>
+    </row>
+    <row r="21" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M21" s="12">
         <v>-8.6</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="10">
         <f t="shared" si="0"/>
         <v>46.599999999999994</v>
       </c>
-      <c r="O21" s="23">
+      <c r="O21" s="11">
         <f t="shared" si="1"/>
         <v>-8.6</v>
       </c>
-    </row>
-    <row r="22" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M22" s="24">
+      <c r="P21" s="26">
+        <f t="shared" si="2"/>
+        <v>59.759999999999991</v>
+      </c>
+    </row>
+    <row r="22" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M22" s="12">
         <v>-8.4000000000000092</v>
       </c>
-      <c r="N22" s="21">
+      <c r="N22" s="10">
         <f t="shared" si="0"/>
         <v>45.400000000000055</v>
       </c>
-      <c r="O22" s="23">
+      <c r="O22" s="11">
         <f t="shared" si="1"/>
         <v>-8.4000000000000092</v>
       </c>
-    </row>
-    <row r="23" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M23" s="24">
+      <c r="P22" s="26">
+        <f t="shared" si="2"/>
+        <v>56.76000000000014</v>
+      </c>
+    </row>
+    <row r="23" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M23" s="12">
         <v>-8.2000000000000099</v>
       </c>
-      <c r="N23" s="21">
+      <c r="N23" s="10">
         <f t="shared" si="0"/>
         <v>44.20000000000006</v>
       </c>
-      <c r="O23" s="23">
+      <c r="O23" s="11">
         <f t="shared" si="1"/>
         <v>-8.2000000000000099</v>
       </c>
-    </row>
-    <row r="24" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M24" s="24">
+      <c r="P23" s="26">
+        <f t="shared" si="2"/>
+        <v>53.840000000000146</v>
+      </c>
+    </row>
+    <row r="24" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M24" s="12">
         <v>-8.0000000000000107</v>
       </c>
-      <c r="N24" s="21">
+      <c r="N24" s="10">
         <f t="shared" si="0"/>
         <v>43.000000000000064</v>
       </c>
-      <c r="O24" s="23">
+      <c r="O24" s="11">
         <f t="shared" si="1"/>
         <v>-8.0000000000000107</v>
       </c>
-    </row>
-    <row r="25" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M25" s="24">
+      <c r="P24" s="26">
+        <f t="shared" si="2"/>
+        <v>51.000000000000149</v>
+      </c>
+    </row>
+    <row r="25" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M25" s="12">
         <v>-7.8000000000000096</v>
       </c>
-      <c r="N25" s="21">
+      <c r="N25" s="10">
         <f t="shared" si="0"/>
         <v>41.800000000000054</v>
       </c>
-      <c r="O25" s="23">
+      <c r="O25" s="11">
         <f t="shared" si="1"/>
         <v>-7.8000000000000096</v>
       </c>
-    </row>
-    <row r="26" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M26" s="24">
+      <c r="P25" s="26">
+        <f t="shared" si="2"/>
+        <v>48.240000000000137</v>
+      </c>
+    </row>
+    <row r="26" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M26" s="12">
         <v>-7.6000000000000103</v>
       </c>
-      <c r="N26" s="21">
+      <c r="N26" s="10">
         <f t="shared" si="0"/>
         <v>40.600000000000065</v>
       </c>
-      <c r="O26" s="23">
+      <c r="O26" s="11">
         <f t="shared" si="1"/>
         <v>-7.6000000000000103</v>
       </c>
-    </row>
-    <row r="27" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M27" s="24">
+      <c r="P26" s="26">
+        <f t="shared" si="2"/>
+        <v>45.56000000000013</v>
+      </c>
+    </row>
+    <row r="27" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M27" s="12">
         <v>-7.4000000000000101</v>
       </c>
-      <c r="N27" s="21">
+      <c r="N27" s="10">
         <f t="shared" si="0"/>
         <v>39.400000000000063</v>
       </c>
-      <c r="O27" s="23">
+      <c r="O27" s="11">
         <f t="shared" si="1"/>
         <v>-7.4000000000000101</v>
       </c>
-    </row>
-    <row r="28" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M28" s="24">
+      <c r="P27" s="26">
+        <f t="shared" si="2"/>
+        <v>42.960000000000129</v>
+      </c>
+    </row>
+    <row r="28" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M28" s="12">
         <v>-7.2000000000000099</v>
       </c>
-      <c r="N28" s="21">
+      <c r="N28" s="10">
         <f t="shared" si="0"/>
         <v>38.20000000000006</v>
       </c>
-      <c r="O28" s="23">
+      <c r="O28" s="11">
         <f t="shared" si="1"/>
         <v>-7.2000000000000099</v>
       </c>
-    </row>
-    <row r="29" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M29" s="24">
+      <c r="P28" s="26">
+        <f t="shared" si="2"/>
+        <v>40.440000000000126</v>
+      </c>
+    </row>
+    <row r="29" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M29" s="12">
         <v>-7.0000000000000098</v>
       </c>
-      <c r="N29" s="21">
+      <c r="N29" s="10">
         <f t="shared" si="0"/>
         <v>37.000000000000057</v>
       </c>
-      <c r="O29" s="23">
+      <c r="O29" s="11">
         <f t="shared" si="1"/>
         <v>-7.0000000000000098</v>
       </c>
-    </row>
-    <row r="30" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M30" s="24">
+      <c r="P29" s="26">
+        <f t="shared" si="2"/>
+        <v>38.000000000000114</v>
+      </c>
+    </row>
+    <row r="30" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M30" s="12">
         <v>-6.8000000000000096</v>
       </c>
-      <c r="N30" s="21">
+      <c r="N30" s="10">
         <f t="shared" si="0"/>
         <v>35.800000000000054</v>
       </c>
-      <c r="O30" s="23">
+      <c r="O30" s="11">
         <f t="shared" si="1"/>
         <v>-6.8000000000000096</v>
       </c>
-    </row>
-    <row r="31" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M31" s="24">
+      <c r="P30" s="26">
+        <f t="shared" si="2"/>
+        <v>35.640000000000114</v>
+      </c>
+    </row>
+    <row r="31" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M31" s="12">
         <v>-6.6000000000000103</v>
       </c>
-      <c r="N31" s="21">
+      <c r="N31" s="10">
         <f t="shared" si="0"/>
         <v>34.600000000000065</v>
       </c>
-      <c r="O31" s="23">
+      <c r="O31" s="11">
         <f t="shared" si="1"/>
         <v>-6.6000000000000103</v>
       </c>
-    </row>
-    <row r="32" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M32" s="24">
+      <c r="P31" s="26">
+        <f t="shared" si="2"/>
+        <v>33.360000000000113</v>
+      </c>
+    </row>
+    <row r="32" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M32" s="12">
         <v>-6.4000000000000101</v>
       </c>
-      <c r="N32" s="21">
+      <c r="N32" s="10">
         <f t="shared" si="0"/>
         <v>33.400000000000063</v>
       </c>
-      <c r="O32" s="23">
+      <c r="O32" s="11">
         <f t="shared" si="1"/>
         <v>-6.4000000000000101</v>
       </c>
-    </row>
-    <row r="33" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M33" s="24">
+      <c r="P32" s="26">
+        <f t="shared" si="2"/>
+        <v>31.16000000000011</v>
+      </c>
+    </row>
+    <row r="33" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M33" s="12">
         <v>-6.2000000000000099</v>
       </c>
-      <c r="N33" s="21">
+      <c r="N33" s="10">
         <f t="shared" si="0"/>
         <v>32.20000000000006</v>
       </c>
-      <c r="O33" s="23">
+      <c r="O33" s="11">
         <f t="shared" si="1"/>
         <v>-6.2000000000000099</v>
       </c>
-    </row>
-    <row r="34" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M34" s="24">
+      <c r="P33" s="26">
+        <f t="shared" si="2"/>
+        <v>29.040000000000106</v>
+      </c>
+    </row>
+    <row r="34" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M34" s="12">
         <v>-6.0000000000000098</v>
       </c>
-      <c r="N34" s="21">
+      <c r="N34" s="10">
         <f t="shared" si="0"/>
         <v>31.000000000000057</v>
       </c>
-      <c r="O34" s="23">
+      <c r="O34" s="11">
         <f t="shared" si="1"/>
         <v>-6.0000000000000098</v>
       </c>
-    </row>
-    <row r="35" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M35" s="24">
+      <c r="P34" s="26">
+        <f t="shared" si="2"/>
+        <v>27.000000000000092</v>
+      </c>
+    </row>
+    <row r="35" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M35" s="12">
         <v>-5.8000000000000096</v>
       </c>
-      <c r="N35" s="21">
+      <c r="N35" s="10">
         <f t="shared" si="0"/>
         <v>29.800000000000058</v>
       </c>
-      <c r="O35" s="23">
+      <c r="O35" s="11">
         <f t="shared" si="1"/>
         <v>-5.8000000000000096</v>
       </c>
-    </row>
-    <row r="36" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M36" s="24">
+      <c r="P35" s="26">
+        <f t="shared" si="2"/>
+        <v>25.040000000000095</v>
+      </c>
+    </row>
+    <row r="36" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M36" s="12">
         <v>-5.6000000000000201</v>
       </c>
-      <c r="N36" s="21">
+      <c r="N36" s="10">
         <f t="shared" si="0"/>
         <v>28.600000000000122</v>
       </c>
-      <c r="O36" s="23">
+      <c r="O36" s="11">
         <f t="shared" si="1"/>
         <v>-5.6000000000000201</v>
       </c>
-    </row>
-    <row r="37" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M37" s="24">
+      <c r="P36" s="26">
+        <f t="shared" si="2"/>
+        <v>23.160000000000181</v>
+      </c>
+    </row>
+    <row r="37" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M37" s="12">
         <v>-5.4000000000000199</v>
       </c>
-      <c r="N37" s="21">
+      <c r="N37" s="10">
         <f t="shared" si="0"/>
         <v>27.400000000000119</v>
       </c>
-      <c r="O37" s="23">
+      <c r="O37" s="11">
         <f t="shared" si="1"/>
         <v>-5.4000000000000199</v>
       </c>
-    </row>
-    <row r="38" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M38" s="24">
+      <c r="P37" s="26">
+        <f t="shared" si="2"/>
+        <v>21.360000000000174</v>
+      </c>
+    </row>
+    <row r="38" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M38" s="12">
         <v>-5.2000000000000197</v>
       </c>
-      <c r="N38" s="21">
+      <c r="N38" s="10">
         <f t="shared" si="0"/>
         <v>26.200000000000117</v>
       </c>
-      <c r="O38" s="23">
+      <c r="O38" s="11">
         <f t="shared" si="1"/>
         <v>-5.2000000000000197</v>
       </c>
-    </row>
-    <row r="39" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M39" s="24">
+      <c r="P38" s="26">
+        <f t="shared" si="2"/>
+        <v>19.640000000000164</v>
+      </c>
+    </row>
+    <row r="39" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M39" s="12">
         <v>-5.0000000000000204</v>
       </c>
-      <c r="N39" s="21">
+      <c r="N39" s="10">
         <f t="shared" si="0"/>
         <v>25.000000000000121</v>
       </c>
-      <c r="O39" s="23">
+      <c r="O39" s="11">
         <f t="shared" si="1"/>
         <v>-5.0000000000000204</v>
       </c>
-    </row>
-    <row r="40" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M40" s="24">
+      <c r="P39" s="26">
+        <f t="shared" si="2"/>
+        <v>18.000000000000163</v>
+      </c>
+    </row>
+    <row r="40" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M40" s="12">
         <v>-4.8000000000000203</v>
       </c>
-      <c r="N40" s="21">
+      <c r="N40" s="10">
         <f t="shared" si="0"/>
         <v>23.800000000000122</v>
       </c>
-      <c r="O40" s="23">
+      <c r="O40" s="11">
         <f t="shared" si="1"/>
         <v>-4.8000000000000203</v>
       </c>
-    </row>
-    <row r="41" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M41" s="24">
+      <c r="P40" s="26">
+        <f t="shared" si="2"/>
+        <v>16.440000000000154</v>
+      </c>
+    </row>
+    <row r="41" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M41" s="12">
         <v>-4.6000000000000201</v>
       </c>
-      <c r="N41" s="21">
+      <c r="N41" s="10">
         <f t="shared" si="0"/>
         <v>22.600000000000122</v>
       </c>
-      <c r="O41" s="23">
+      <c r="O41" s="11">
         <f t="shared" si="1"/>
         <v>-4.6000000000000201</v>
       </c>
-    </row>
-    <row r="42" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M42" s="24">
+      <c r="P41" s="26">
+        <f t="shared" si="2"/>
+        <v>14.960000000000145</v>
+      </c>
+    </row>
+    <row r="42" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M42" s="12">
         <v>-4.4000000000000199</v>
       </c>
-      <c r="N42" s="21">
+      <c r="N42" s="10">
         <f t="shared" si="0"/>
         <v>21.400000000000119</v>
       </c>
-      <c r="O42" s="23">
+      <c r="O42" s="11">
         <f t="shared" si="1"/>
         <v>-4.4000000000000199</v>
       </c>
-    </row>
-    <row r="43" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M43" s="24">
+      <c r="P42" s="26">
+        <f t="shared" si="2"/>
+        <v>13.560000000000134</v>
+      </c>
+    </row>
+    <row r="43" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M43" s="12">
         <v>-4.2000000000000197</v>
       </c>
-      <c r="N43" s="21">
+      <c r="N43" s="10">
         <f t="shared" si="0"/>
         <v>20.200000000000117</v>
       </c>
-      <c r="O43" s="23">
+      <c r="O43" s="11">
         <f t="shared" si="1"/>
         <v>-4.2000000000000197</v>
       </c>
-    </row>
-    <row r="44" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M44" s="24">
+      <c r="P43" s="26">
+        <f t="shared" si="2"/>
+        <v>12.240000000000125</v>
+      </c>
+    </row>
+    <row r="44" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M44" s="12">
         <v>-4.0000000000000204</v>
       </c>
-      <c r="N44" s="21">
+      <c r="N44" s="10">
         <f t="shared" si="0"/>
         <v>19.000000000000121</v>
       </c>
-      <c r="O44" s="23">
+      <c r="O44" s="11">
         <f t="shared" si="1"/>
         <v>-4.0000000000000204</v>
       </c>
-    </row>
-    <row r="45" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M45" s="24">
+      <c r="P44" s="26">
+        <f t="shared" si="2"/>
+        <v>11.000000000000123</v>
+      </c>
+    </row>
+    <row r="45" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M45" s="12">
         <v>-3.8000000000000198</v>
       </c>
-      <c r="N45" s="21">
+      <c r="N45" s="10">
         <f t="shared" si="0"/>
         <v>17.800000000000118</v>
       </c>
-      <c r="O45" s="23">
+      <c r="O45" s="11">
         <f t="shared" si="1"/>
         <v>-3.8000000000000198</v>
       </c>
-    </row>
-    <row r="46" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M46" s="24">
+      <c r="P45" s="26">
+        <f t="shared" si="2"/>
+        <v>9.84000000000011</v>
+      </c>
+    </row>
+    <row r="46" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M46" s="12">
         <v>-3.6000000000000201</v>
       </c>
-      <c r="N46" s="21">
+      <c r="N46" s="10">
         <f t="shared" si="0"/>
         <v>16.600000000000122</v>
       </c>
-      <c r="O46" s="23">
+      <c r="O46" s="11">
         <f t="shared" si="1"/>
         <v>-3.6000000000000201</v>
       </c>
-    </row>
-    <row r="47" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M47" s="24">
+      <c r="P46" s="26">
+        <f t="shared" si="2"/>
+        <v>8.7600000000001046</v>
+      </c>
+    </row>
+    <row r="47" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M47" s="12">
         <v>-3.4000000000000199</v>
       </c>
-      <c r="N47" s="21">
+      <c r="N47" s="10">
         <f t="shared" si="0"/>
         <v>15.400000000000119</v>
       </c>
-      <c r="O47" s="23">
+      <c r="O47" s="11">
         <f t="shared" si="1"/>
         <v>-3.4000000000000199</v>
       </c>
-    </row>
-    <row r="48" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M48" s="24">
+      <c r="P47" s="26">
+        <f t="shared" si="2"/>
+        <v>7.7600000000000957</v>
+      </c>
+    </row>
+    <row r="48" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M48" s="12">
         <v>-3.2000000000000202</v>
       </c>
-      <c r="N48" s="21">
+      <c r="N48" s="10">
         <f t="shared" si="0"/>
         <v>14.20000000000012</v>
       </c>
-      <c r="O48" s="23">
+      <c r="O48" s="11">
         <f t="shared" si="1"/>
         <v>-3.2000000000000202</v>
       </c>
-    </row>
-    <row r="49" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M49" s="24">
+      <c r="P48" s="26">
+        <f t="shared" si="2"/>
+        <v>6.8400000000000896</v>
+      </c>
+    </row>
+    <row r="49" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M49" s="12">
         <v>-3.00000000000002</v>
       </c>
-      <c r="N49" s="21">
+      <c r="N49" s="10">
         <f t="shared" si="0"/>
         <v>13.000000000000121</v>
       </c>
-      <c r="O49" s="23">
+      <c r="O49" s="11">
         <f t="shared" si="1"/>
         <v>-3.00000000000002</v>
       </c>
-    </row>
-    <row r="50" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M50" s="24">
+      <c r="P49" s="26">
+        <f t="shared" si="2"/>
+        <v>6.0000000000000808</v>
+      </c>
+    </row>
+    <row r="50" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M50" s="12">
         <v>-2.80000000000003</v>
       </c>
-      <c r="N50" s="21">
+      <c r="N50" s="10">
         <f t="shared" si="0"/>
         <v>11.80000000000018</v>
       </c>
-      <c r="O50" s="23">
+      <c r="O50" s="11">
         <f t="shared" si="1"/>
         <v>-2.80000000000003</v>
       </c>
-    </row>
-    <row r="51" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M51" s="24">
+      <c r="P50" s="26">
+        <f t="shared" si="2"/>
+        <v>5.2400000000001077</v>
+      </c>
+    </row>
+    <row r="51" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M51" s="12">
         <v>-2.6000000000000298</v>
       </c>
-      <c r="N51" s="21">
+      <c r="N51" s="10">
         <f t="shared" si="0"/>
         <v>10.600000000000179</v>
       </c>
-      <c r="O51" s="23">
+      <c r="O51" s="11">
         <f t="shared" si="1"/>
         <v>-2.6000000000000298</v>
       </c>
-    </row>
-    <row r="52" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M52" s="24">
+      <c r="P51" s="26">
+        <f t="shared" si="2"/>
+        <v>4.5600000000000955</v>
+      </c>
+    </row>
+    <row r="52" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M52" s="12">
         <v>-2.4000000000000301</v>
       </c>
-      <c r="N52" s="21">
+      <c r="N52" s="10">
         <f t="shared" si="0"/>
         <v>9.4000000000001798</v>
       </c>
-      <c r="O52" s="23">
+      <c r="O52" s="11">
         <f t="shared" si="1"/>
         <v>-2.4000000000000301</v>
       </c>
-    </row>
-    <row r="53" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M53" s="24">
+      <c r="P52" s="26">
+        <f t="shared" si="2"/>
+        <v>3.9600000000000843</v>
+      </c>
+    </row>
+    <row r="53" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M53" s="12">
         <v>-2.2000000000000299</v>
       </c>
-      <c r="N53" s="21">
+      <c r="N53" s="10">
         <f t="shared" si="0"/>
         <v>8.2000000000001805</v>
       </c>
-      <c r="O53" s="23">
+      <c r="O53" s="11">
         <f t="shared" si="1"/>
         <v>-2.2000000000000299</v>
       </c>
-    </row>
-    <row r="54" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M54" s="24">
+      <c r="P53" s="26">
+        <f t="shared" si="2"/>
+        <v>3.4400000000000714</v>
+      </c>
+    </row>
+    <row r="54" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M54" s="12">
         <v>-2.0000000000000302</v>
       </c>
-      <c r="N54" s="21">
+      <c r="N54" s="10">
         <f t="shared" si="0"/>
         <v>7.0000000000001812</v>
       </c>
-      <c r="O54" s="23">
+      <c r="O54" s="11">
         <f t="shared" si="1"/>
         <v>-2.0000000000000302</v>
       </c>
-    </row>
-    <row r="55" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M55" s="24">
+      <c r="P54" s="26">
+        <f t="shared" si="2"/>
+        <v>3.0000000000000604</v>
+      </c>
+    </row>
+    <row r="55" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M55" s="12">
         <v>-1.80000000000003</v>
       </c>
-      <c r="N55" s="21">
+      <c r="N55" s="10">
         <f t="shared" si="0"/>
         <v>5.8000000000001801</v>
       </c>
-      <c r="O55" s="23">
+      <c r="O55" s="11">
         <f t="shared" si="1"/>
         <v>-1.80000000000003</v>
       </c>
-    </row>
-    <row r="56" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M56" s="24">
+      <c r="P55" s="26">
+        <f t="shared" si="2"/>
+        <v>2.6400000000000481</v>
+      </c>
+    </row>
+    <row r="56" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M56" s="12">
         <v>-1.6000000000000301</v>
       </c>
-      <c r="N56" s="21">
+      <c r="N56" s="10">
         <f t="shared" si="0"/>
         <v>4.6000000000001808</v>
       </c>
-      <c r="O56" s="23">
+      <c r="O56" s="11">
         <f t="shared" si="1"/>
         <v>-1.6000000000000301</v>
       </c>
-    </row>
-    <row r="57" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M57" s="24">
+      <c r="P56" s="26">
+        <f t="shared" si="2"/>
+        <v>2.3600000000000363</v>
+      </c>
+    </row>
+    <row r="57" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M57" s="12">
         <v>-1.4000000000000301</v>
       </c>
-      <c r="N57" s="21">
+      <c r="N57" s="10">
         <f t="shared" si="0"/>
         <v>4.5999999999998193</v>
       </c>
-      <c r="O57" s="23">
+      <c r="O57" s="11">
         <f t="shared" si="1"/>
         <v>-1.4000000000000301</v>
       </c>
-    </row>
-    <row r="58" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M58" s="24">
+      <c r="P57" s="26">
+        <f t="shared" si="2"/>
+        <v>2.1600000000000241</v>
+      </c>
+    </row>
+    <row r="58" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M58" s="12">
         <v>-1.2000000000000299</v>
       </c>
-      <c r="N58" s="21">
+      <c r="N58" s="10">
         <f t="shared" si="0"/>
         <v>5.7999999999998204</v>
       </c>
-      <c r="O58" s="23">
+      <c r="O58" s="11">
         <f t="shared" si="1"/>
         <v>-1.2000000000000299</v>
       </c>
-    </row>
-    <row r="59" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M59" s="24">
+      <c r="P58" s="26">
+        <f t="shared" si="2"/>
+        <v>2.040000000000012</v>
+      </c>
+    </row>
+    <row r="59" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M59" s="12">
         <v>-1.00000000000003</v>
       </c>
-      <c r="N59" s="21">
+      <c r="N59" s="10">
         <f t="shared" si="0"/>
         <v>6.9999999999998206</v>
       </c>
-      <c r="O59" s="23">
+      <c r="O59" s="11">
         <f t="shared" si="1"/>
         <v>-1.00000000000003</v>
       </c>
-    </row>
-    <row r="60" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M60" s="24">
+      <c r="P59" s="26">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M60" s="12">
         <v>-0.80000000000002902</v>
       </c>
-      <c r="N60" s="21">
+      <c r="N60" s="10">
         <f t="shared" si="0"/>
         <v>8.1999999999998252</v>
       </c>
-      <c r="O60" s="23">
+      <c r="O60" s="11">
         <f t="shared" si="1"/>
         <v>-0.80000000000002902</v>
       </c>
-    </row>
-    <row r="61" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M61" s="24">
+      <c r="P60" s="26">
+        <f t="shared" si="2"/>
+        <v>2.0399999999999885</v>
+      </c>
+    </row>
+    <row r="61" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M61" s="12">
         <v>-0.60000000000002995</v>
       </c>
-      <c r="N61" s="21">
+      <c r="N61" s="10">
         <f t="shared" si="0"/>
         <v>9.3999999999998209</v>
       </c>
-      <c r="O61" s="23">
+      <c r="O61" s="11">
         <f t="shared" si="1"/>
         <v>-0.60000000000002995</v>
       </c>
-    </row>
-    <row r="62" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M62" s="24">
+      <c r="P61" s="26">
+        <f t="shared" si="2"/>
+        <v>2.1599999999999762</v>
+      </c>
+    </row>
+    <row r="62" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M62" s="12">
         <v>-0.400000000000031</v>
       </c>
-      <c r="N62" s="21">
+      <c r="N62" s="10">
         <f t="shared" si="0"/>
         <v>10.599999999999813</v>
       </c>
-      <c r="O62" s="23">
+      <c r="O62" s="11">
         <f t="shared" si="1"/>
         <v>-0.400000000000031</v>
       </c>
-    </row>
-    <row r="63" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M63" s="24">
+      <c r="P62" s="26">
+        <f t="shared" si="2"/>
+        <v>2.359999999999963</v>
+      </c>
+    </row>
+    <row r="63" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M63" s="12">
         <v>-0.20000000000002899</v>
       </c>
-      <c r="N63" s="21">
+      <c r="N63" s="10">
         <f t="shared" si="0"/>
         <v>11.799999999999827</v>
       </c>
-      <c r="O63" s="23">
+      <c r="O63" s="11">
         <f t="shared" si="1"/>
         <v>-0.20000000000002899</v>
       </c>
-    </row>
-    <row r="64" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M64" s="24">
+      <c r="P63" s="26">
+        <f t="shared" si="2"/>
+        <v>2.6399999999999535</v>
+      </c>
+    </row>
+    <row r="64" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M64" s="12">
         <v>-4.0856207306205799E-14</v>
       </c>
-      <c r="N64" s="21">
+      <c r="N64" s="10">
         <f t="shared" si="0"/>
         <v>12.999999999999755</v>
       </c>
-      <c r="O64" s="23">
+      <c r="O64" s="11">
         <f t="shared" si="1"/>
         <v>-4.0856207306205799E-14</v>
       </c>
-    </row>
-    <row r="65" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M65" s="24">
+      <c r="P64" s="26">
+        <f t="shared" si="2"/>
+        <v>2.9999999999999183</v>
+      </c>
+    </row>
+    <row r="65" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M65" s="12">
         <v>0.19999999999999901</v>
       </c>
-      <c r="N65" s="21">
+      <c r="N65" s="10">
         <f t="shared" si="0"/>
         <v>14.199999999999994</v>
       </c>
-      <c r="O65" s="23">
+      <c r="O65" s="11">
         <f t="shared" si="1"/>
         <v>0.19999999999999901</v>
       </c>
-    </row>
-    <row r="66" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M66" s="24">
+      <c r="P65" s="26">
+        <f t="shared" si="2"/>
+        <v>3.4399999999999977</v>
+      </c>
+    </row>
+    <row r="66" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M66" s="12">
         <v>0.4</v>
       </c>
-      <c r="N66" s="21">
+      <c r="N66" s="10">
         <f t="shared" si="0"/>
         <v>15.399999999999999</v>
       </c>
-      <c r="O66" s="23">
+      <c r="O66" s="11">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="67" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M67" s="24">
+      <c r="P66" s="26">
+        <f t="shared" si="2"/>
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="67" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M67" s="12">
         <v>0.6</v>
       </c>
-      <c r="N67" s="21">
+      <c r="N67" s="10">
         <f t="shared" si="0"/>
         <v>16.600000000000001</v>
       </c>
-      <c r="O67" s="23">
+      <c r="O67" s="11">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="68" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M68" s="24">
+      <c r="P67" s="26">
+        <f t="shared" si="2"/>
+        <v>4.5600000000000005</v>
+      </c>
+    </row>
+    <row r="68" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M68" s="12">
         <v>0.80000000000000104</v>
       </c>
-      <c r="N68" s="21">
+      <c r="N68" s="10">
         <f t="shared" si="0"/>
         <v>17.800000000000008</v>
       </c>
-      <c r="O68" s="23">
+      <c r="O68" s="11">
         <f t="shared" si="1"/>
         <v>0.80000000000000104</v>
       </c>
-    </row>
-    <row r="69" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M69" s="24">
+      <c r="P68" s="26">
+        <f t="shared" si="2"/>
+        <v>5.2400000000000038</v>
+      </c>
+    </row>
+    <row r="69" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M69" s="12">
         <v>1</v>
       </c>
-      <c r="N69" s="21">
+      <c r="N69" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="O69" s="23">
+      <c r="O69" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M70" s="24">
+      <c r="P69" s="26">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M70" s="12">
         <v>1.2</v>
       </c>
-      <c r="N70" s="21">
+      <c r="N70" s="10">
         <f t="shared" si="0"/>
         <v>20.200000000000003</v>
       </c>
-      <c r="O70" s="23">
+      <c r="O70" s="11">
         <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
-    </row>
-    <row r="71" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M71" s="24">
+      <c r="P70" s="26">
+        <f t="shared" si="2"/>
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="71" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M71" s="12">
         <v>1.4</v>
       </c>
-      <c r="N71" s="21">
+      <c r="N71" s="10">
         <f t="shared" si="0"/>
         <v>21.4</v>
       </c>
-      <c r="O71" s="23">
+      <c r="O71" s="11">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-    </row>
-    <row r="72" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M72" s="24">
+      <c r="P71" s="26">
+        <f t="shared" si="2"/>
+        <v>7.76</v>
+      </c>
+    </row>
+    <row r="72" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M72" s="12">
         <v>1.6</v>
       </c>
-      <c r="N72" s="21">
+      <c r="N72" s="10">
         <f t="shared" si="0"/>
         <v>22.6</v>
       </c>
-      <c r="O72" s="23">
+      <c r="O72" s="11">
         <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="73" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M73" s="24">
+      <c r="P72" s="26">
+        <f t="shared" si="2"/>
+        <v>8.7600000000000016</v>
+      </c>
+    </row>
+    <row r="73" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M73" s="12">
         <v>1.8</v>
       </c>
-      <c r="N73" s="21">
+      <c r="N73" s="10">
         <f t="shared" si="0"/>
         <v>23.799999999999997</v>
       </c>
-      <c r="O73" s="23">
+      <c r="O73" s="11">
         <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
-    </row>
-    <row r="74" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M74" s="24">
+      <c r="P73" s="26">
+        <f t="shared" si="2"/>
+        <v>9.84</v>
+      </c>
+    </row>
+    <row r="74" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M74" s="12">
         <v>2</v>
       </c>
-      <c r="N74" s="21">
+      <c r="N74" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="O74" s="23">
+      <c r="O74" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M75" s="24">
+      <c r="P74" s="26">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M75" s="12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N75" s="21">
+      <c r="N75" s="10">
         <f t="shared" si="0"/>
         <v>26.200000000000003</v>
       </c>
-      <c r="O75" s="23">
+      <c r="O75" s="11">
         <f t="shared" si="1"/>
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M76" s="24">
+      <c r="P75" s="26">
+        <f t="shared" si="2"/>
+        <v>12.240000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M76" s="12">
         <v>2.4</v>
       </c>
-      <c r="N76" s="21">
+      <c r="N76" s="10">
         <f t="shared" si="0"/>
         <v>27.4</v>
       </c>
-      <c r="O76" s="23">
+      <c r="O76" s="11">
         <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
-    </row>
-    <row r="77" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M77" s="24">
+      <c r="P76" s="26">
+        <f t="shared" si="2"/>
+        <v>13.559999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M77" s="12">
         <v>2.6</v>
       </c>
-      <c r="N77" s="21">
+      <c r="N77" s="10">
         <f t="shared" si="0"/>
         <v>28.599999999999998</v>
       </c>
-      <c r="O77" s="23">
+      <c r="O77" s="11">
         <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
-    </row>
-    <row r="78" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M78" s="24">
+      <c r="P77" s="26">
+        <f t="shared" si="2"/>
+        <v>14.96</v>
+      </c>
+    </row>
+    <row r="78" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M78" s="12">
         <v>2.8</v>
       </c>
-      <c r="N78" s="21">
+      <c r="N78" s="10">
         <f t="shared" si="0"/>
         <v>29.799999999999997</v>
       </c>
-      <c r="O78" s="23">
+      <c r="O78" s="11">
         <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
-    </row>
-    <row r="79" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M79" s="24">
+      <c r="P78" s="26">
+        <f t="shared" si="2"/>
+        <v>16.439999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M79" s="12">
         <v>3</v>
       </c>
-      <c r="N79" s="21">
-        <f t="shared" ref="N79:N114" si="2">$F$6*ABS($G$6*M79+$H$6)+$I$6</f>
+      <c r="N79" s="10">
+        <f t="shared" ref="N79:N114" si="3">$F$6*ABS($G$6*M79+$H$6)+$I$6</f>
         <v>31</v>
       </c>
-      <c r="O79" s="23">
-        <f t="shared" ref="O79:O114" si="3">$F$7*M79+G72</f>
+      <c r="O79" s="11">
+        <f t="shared" ref="O79:O114" si="4">$F$7*M79+G72</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M80" s="24">
+      <c r="P79" s="26">
+        <f t="shared" ref="P79:P114" si="5">$F$8*(M79^2)+$G$8*M79+$H$8</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M80" s="12">
         <v>3.2</v>
       </c>
-      <c r="N80" s="21">
-        <f t="shared" si="2"/>
+      <c r="N80" s="10">
+        <f t="shared" si="3"/>
         <v>32.200000000000003</v>
       </c>
-      <c r="O80" s="23">
+      <c r="O80" s="11">
+        <f t="shared" si="4"/>
+        <v>3.2</v>
+      </c>
+      <c r="P80" s="26">
+        <f t="shared" si="5"/>
+        <v>19.64</v>
+      </c>
+    </row>
+    <row r="81" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M81" s="12">
+        <v>3.4</v>
+      </c>
+      <c r="N81" s="10">
         <f t="shared" si="3"/>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="81" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M81" s="24">
+        <v>33.400000000000006</v>
+      </c>
+      <c r="O81" s="11">
+        <f t="shared" si="4"/>
         <v>3.4</v>
       </c>
-      <c r="N81" s="21">
-        <f t="shared" si="2"/>
-        <v>33.400000000000006</v>
-      </c>
-      <c r="O81" s="23">
+      <c r="P81" s="26">
+        <f t="shared" si="5"/>
+        <v>21.36</v>
+      </c>
+    </row>
+    <row r="82" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M82" s="12">
+        <v>3.6</v>
+      </c>
+      <c r="N82" s="10">
         <f t="shared" si="3"/>
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="82" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M82" s="24">
+        <v>34.599999999999994</v>
+      </c>
+      <c r="O82" s="11">
+        <f t="shared" si="4"/>
         <v>3.6</v>
       </c>
-      <c r="N82" s="21">
-        <f t="shared" si="2"/>
-        <v>34.599999999999994</v>
-      </c>
-      <c r="O82" s="23">
+      <c r="P82" s="26">
+        <f t="shared" si="5"/>
+        <v>23.16</v>
+      </c>
+    </row>
+    <row r="83" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M83" s="12">
+        <v>3.8</v>
+      </c>
+      <c r="N83" s="10">
         <f t="shared" si="3"/>
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="83" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M83" s="24">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="O83" s="11">
+        <f t="shared" si="4"/>
         <v>3.8</v>
       </c>
-      <c r="N83" s="21">
-        <f t="shared" si="2"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="O83" s="23">
+      <c r="P83" s="26">
+        <f t="shared" si="5"/>
+        <v>25.04</v>
+      </c>
+    </row>
+    <row r="84" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M84" s="12">
+        <v>4</v>
+      </c>
+      <c r="N84" s="10">
         <f t="shared" si="3"/>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="84" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M84" s="24">
+        <v>37</v>
+      </c>
+      <c r="O84" s="11">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="N84" s="21">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="O84" s="23">
+      <c r="P84" s="26">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M85" s="12">
+        <v>4.1999999999998998</v>
+      </c>
+      <c r="N85" s="10">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M85" s="24">
+        <v>38.199999999999399</v>
+      </c>
+      <c r="O85" s="11">
+        <f t="shared" si="4"/>
         <v>4.1999999999998998</v>
       </c>
-      <c r="N85" s="21">
-        <f t="shared" si="2"/>
-        <v>38.199999999999399</v>
-      </c>
-      <c r="O85" s="23">
+      <c r="P85" s="26">
+        <f t="shared" si="5"/>
+        <v>29.039999999998958</v>
+      </c>
+    </row>
+    <row r="86" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M86" s="12">
+        <v>4.3999999999999</v>
+      </c>
+      <c r="N86" s="10">
         <f t="shared" si="3"/>
-        <v>4.1999999999998998</v>
-      </c>
-    </row>
-    <row r="86" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M86" s="24">
+        <v>39.399999999999402</v>
+      </c>
+      <c r="O86" s="11">
+        <f t="shared" si="4"/>
         <v>4.3999999999999</v>
       </c>
-      <c r="N86" s="21">
-        <f t="shared" si="2"/>
-        <v>39.399999999999402</v>
-      </c>
-      <c r="O86" s="23">
+      <c r="P86" s="26">
+        <f t="shared" si="5"/>
+        <v>31.159999999998917</v>
+      </c>
+    </row>
+    <row r="87" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M87" s="12">
+        <v>4.5999999999999002</v>
+      </c>
+      <c r="N87" s="10">
         <f t="shared" si="3"/>
-        <v>4.3999999999999</v>
-      </c>
-    </row>
-    <row r="87" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M87" s="24">
+        <v>40.599999999999397</v>
+      </c>
+      <c r="O87" s="11">
+        <f t="shared" si="4"/>
         <v>4.5999999999999002</v>
       </c>
-      <c r="N87" s="21">
-        <f t="shared" si="2"/>
-        <v>40.599999999999397</v>
-      </c>
-      <c r="O87" s="23">
+      <c r="P87" s="26">
+        <f t="shared" si="5"/>
+        <v>33.359999999998877</v>
+      </c>
+    </row>
+    <row r="88" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M88" s="12">
+        <v>4.7999999999999003</v>
+      </c>
+      <c r="N88" s="10">
         <f t="shared" si="3"/>
-        <v>4.5999999999999002</v>
-      </c>
-    </row>
-    <row r="88" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M88" s="24">
+        <v>41.7999999999994</v>
+      </c>
+      <c r="O88" s="11">
+        <f t="shared" si="4"/>
         <v>4.7999999999999003</v>
       </c>
-      <c r="N88" s="21">
-        <f t="shared" si="2"/>
-        <v>41.7999999999994</v>
-      </c>
-      <c r="O88" s="23">
+      <c r="P88" s="26">
+        <f t="shared" si="5"/>
+        <v>35.639999999998842</v>
+      </c>
+    </row>
+    <row r="89" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M89" s="12">
+        <v>4.9999999999998996</v>
+      </c>
+      <c r="N89" s="10">
         <f t="shared" si="3"/>
-        <v>4.7999999999999003</v>
-      </c>
-    </row>
-    <row r="89" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M89" s="24">
+        <v>42.999999999999396</v>
+      </c>
+      <c r="O89" s="11">
+        <f t="shared" si="4"/>
         <v>4.9999999999998996</v>
       </c>
-      <c r="N89" s="21">
-        <f t="shared" si="2"/>
-        <v>42.999999999999396</v>
-      </c>
-      <c r="O89" s="23">
+      <c r="P89" s="26">
+        <f t="shared" si="5"/>
+        <v>37.999999999998799</v>
+      </c>
+    </row>
+    <row r="90" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M90" s="12">
+        <v>5.1999999999998998</v>
+      </c>
+      <c r="N90" s="10">
         <f t="shared" si="3"/>
-        <v>4.9999999999998996</v>
-      </c>
-    </row>
-    <row r="90" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M90" s="24">
+        <v>44.199999999999399</v>
+      </c>
+      <c r="O90" s="11">
+        <f t="shared" si="4"/>
         <v>5.1999999999998998</v>
       </c>
-      <c r="N90" s="21">
-        <f t="shared" si="2"/>
-        <v>44.199999999999399</v>
-      </c>
-      <c r="O90" s="23">
+      <c r="P90" s="26">
+        <f t="shared" si="5"/>
+        <v>40.439999999998761</v>
+      </c>
+    </row>
+    <row r="91" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M91" s="12">
+        <v>5.3999999999999</v>
+      </c>
+      <c r="N91" s="10">
         <f t="shared" si="3"/>
-        <v>5.1999999999998998</v>
-      </c>
-    </row>
-    <row r="91" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M91" s="24">
+        <v>45.399999999999402</v>
+      </c>
+      <c r="O91" s="11">
+        <f t="shared" si="4"/>
         <v>5.3999999999999</v>
       </c>
-      <c r="N91" s="21">
-        <f t="shared" si="2"/>
-        <v>45.399999999999402</v>
-      </c>
-      <c r="O91" s="23">
+      <c r="P91" s="26">
+        <f t="shared" si="5"/>
+        <v>42.959999999998722</v>
+      </c>
+    </row>
+    <row r="92" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M92" s="12">
+        <v>5.5999999999999002</v>
+      </c>
+      <c r="N92" s="10">
         <f t="shared" si="3"/>
-        <v>5.3999999999999</v>
-      </c>
-    </row>
-    <row r="92" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M92" s="24">
+        <v>46.599999999999397</v>
+      </c>
+      <c r="O92" s="11">
+        <f t="shared" si="4"/>
         <v>5.5999999999999002</v>
       </c>
-      <c r="N92" s="21">
-        <f t="shared" si="2"/>
-        <v>46.599999999999397</v>
-      </c>
-      <c r="O92" s="23">
+      <c r="P92" s="26">
+        <f t="shared" si="5"/>
+        <v>45.559999999998681</v>
+      </c>
+    </row>
+    <row r="93" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M93" s="12">
+        <v>5.7999999999999003</v>
+      </c>
+      <c r="N93" s="10">
         <f t="shared" si="3"/>
-        <v>5.5999999999999002</v>
-      </c>
-    </row>
-    <row r="93" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M93" s="24">
+        <v>47.7999999999994</v>
+      </c>
+      <c r="O93" s="11">
+        <f t="shared" si="4"/>
         <v>5.7999999999999003</v>
       </c>
-      <c r="N93" s="21">
-        <f t="shared" si="2"/>
-        <v>47.7999999999994</v>
-      </c>
-      <c r="O93" s="23">
+      <c r="P93" s="26">
+        <f t="shared" si="5"/>
+        <v>48.239999999998645</v>
+      </c>
+    </row>
+    <row r="94" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M94" s="12">
+        <v>5.9999999999998996</v>
+      </c>
+      <c r="N94" s="10">
         <f t="shared" si="3"/>
-        <v>5.7999999999999003</v>
-      </c>
-    </row>
-    <row r="94" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M94" s="24">
+        <v>48.999999999999396</v>
+      </c>
+      <c r="O94" s="11">
+        <f t="shared" si="4"/>
         <v>5.9999999999998996</v>
       </c>
-      <c r="N94" s="21">
-        <f t="shared" si="2"/>
-        <v>48.999999999999396</v>
-      </c>
-      <c r="O94" s="23">
+      <c r="P94" s="26">
+        <f t="shared" si="5"/>
+        <v>50.999999999998593</v>
+      </c>
+    </row>
+    <row r="95" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M95" s="12">
+        <v>6.1999999999998998</v>
+      </c>
+      <c r="N95" s="10">
         <f t="shared" si="3"/>
-        <v>5.9999999999998996</v>
-      </c>
-    </row>
-    <row r="95" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M95" s="24">
+        <v>50.199999999999399</v>
+      </c>
+      <c r="O95" s="11">
+        <f t="shared" si="4"/>
         <v>6.1999999999998998</v>
       </c>
-      <c r="N95" s="21">
-        <f t="shared" si="2"/>
-        <v>50.199999999999399</v>
-      </c>
-      <c r="O95" s="23">
+      <c r="P95" s="26">
+        <f t="shared" si="5"/>
+        <v>53.839999999998554</v>
+      </c>
+    </row>
+    <row r="96" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M96" s="12">
+        <v>6.3999999999999</v>
+      </c>
+      <c r="N96" s="10">
         <f t="shared" si="3"/>
-        <v>6.1999999999998998</v>
-      </c>
-    </row>
-    <row r="96" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M96" s="24">
+        <v>51.399999999999402</v>
+      </c>
+      <c r="O96" s="11">
+        <f t="shared" si="4"/>
         <v>6.3999999999999</v>
       </c>
-      <c r="N96" s="21">
-        <f t="shared" si="2"/>
-        <v>51.399999999999402</v>
-      </c>
-      <c r="O96" s="23">
+      <c r="P96" s="26">
+        <f t="shared" si="5"/>
+        <v>56.75999999999852</v>
+      </c>
+    </row>
+    <row r="97" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M97" s="12">
+        <v>6.5999999999999002</v>
+      </c>
+      <c r="N97" s="10">
         <f t="shared" si="3"/>
-        <v>6.3999999999999</v>
-      </c>
-    </row>
-    <row r="97" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M97" s="24">
+        <v>52.599999999999397</v>
+      </c>
+      <c r="O97" s="11">
+        <f t="shared" si="4"/>
         <v>6.5999999999999002</v>
       </c>
-      <c r="N97" s="21">
-        <f t="shared" si="2"/>
-        <v>52.599999999999397</v>
-      </c>
-      <c r="O97" s="23">
+      <c r="P97" s="26">
+        <f t="shared" si="5"/>
+        <v>59.759999999998485</v>
+      </c>
+    </row>
+    <row r="98" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M98" s="12">
+        <v>6.7999999999999003</v>
+      </c>
+      <c r="N98" s="10">
         <f t="shared" si="3"/>
-        <v>6.5999999999999002</v>
-      </c>
-    </row>
-    <row r="98" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M98" s="24">
+        <v>53.799999999999407</v>
+      </c>
+      <c r="O98" s="11">
+        <f t="shared" si="4"/>
         <v>6.7999999999999003</v>
       </c>
-      <c r="N98" s="21">
-        <f t="shared" si="2"/>
-        <v>53.799999999999407</v>
-      </c>
-      <c r="O98" s="23">
+      <c r="P98" s="26">
+        <f t="shared" si="5"/>
+        <v>62.839999999998447</v>
+      </c>
+    </row>
+    <row r="99" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M99" s="12">
+        <v>6.9999999999998996</v>
+      </c>
+      <c r="N99" s="10">
         <f t="shared" si="3"/>
-        <v>6.7999999999999003</v>
-      </c>
-    </row>
-    <row r="99" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M99" s="24">
+        <v>54.999999999999403</v>
+      </c>
+      <c r="O99" s="11">
+        <f t="shared" si="4"/>
         <v>6.9999999999998996</v>
       </c>
-      <c r="N99" s="21">
-        <f t="shared" si="2"/>
-        <v>54.999999999999403</v>
-      </c>
-      <c r="O99" s="23">
+      <c r="P99" s="26">
+        <f t="shared" si="5"/>
+        <v>65.999999999998394</v>
+      </c>
+    </row>
+    <row r="100" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M100" s="12">
+        <v>7.1999999999998998</v>
+      </c>
+      <c r="N100" s="10">
         <f t="shared" si="3"/>
-        <v>6.9999999999998996</v>
-      </c>
-    </row>
-    <row r="100" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M100" s="24">
+        <v>56.199999999999399</v>
+      </c>
+      <c r="O100" s="11">
+        <f t="shared" si="4"/>
         <v>7.1999999999998998</v>
       </c>
-      <c r="N100" s="21">
-        <f t="shared" si="2"/>
-        <v>56.199999999999399</v>
-      </c>
-      <c r="O100" s="23">
+      <c r="P100" s="26">
+        <f t="shared" si="5"/>
+        <v>69.239999999998361</v>
+      </c>
+    </row>
+    <row r="101" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M101" s="12">
+        <v>7.3999999999999</v>
+      </c>
+      <c r="N101" s="10">
         <f t="shared" si="3"/>
-        <v>7.1999999999998998</v>
-      </c>
-    </row>
-    <row r="101" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M101" s="24">
+        <v>57.399999999999395</v>
+      </c>
+      <c r="O101" s="11">
+        <f t="shared" si="4"/>
         <v>7.3999999999999</v>
       </c>
-      <c r="N101" s="21">
-        <f t="shared" si="2"/>
-        <v>57.399999999999395</v>
-      </c>
-      <c r="O101" s="23">
+      <c r="P101" s="26">
+        <f t="shared" si="5"/>
+        <v>72.559999999998325</v>
+      </c>
+    </row>
+    <row r="102" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M102" s="12">
+        <v>7.5999999999999002</v>
+      </c>
+      <c r="N102" s="10">
         <f t="shared" si="3"/>
-        <v>7.3999999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M102" s="24">
+        <v>58.599999999999397</v>
+      </c>
+      <c r="O102" s="11">
+        <f t="shared" si="4"/>
         <v>7.5999999999999002</v>
       </c>
-      <c r="N102" s="21">
-        <f t="shared" si="2"/>
-        <v>58.599999999999397</v>
-      </c>
-      <c r="O102" s="23">
+      <c r="P102" s="26">
+        <f t="shared" si="5"/>
+        <v>75.959999999998288</v>
+      </c>
+    </row>
+    <row r="103" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M103" s="12">
+        <v>7.7999999999999003</v>
+      </c>
+      <c r="N103" s="10">
         <f t="shared" si="3"/>
-        <v>7.5999999999999002</v>
-      </c>
-    </row>
-    <row r="103" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M103" s="24">
+        <v>59.799999999999407</v>
+      </c>
+      <c r="O103" s="11">
+        <f t="shared" si="4"/>
         <v>7.7999999999999003</v>
       </c>
-      <c r="N103" s="21">
-        <f t="shared" si="2"/>
-        <v>59.799999999999407</v>
-      </c>
-      <c r="O103" s="23">
+      <c r="P103" s="26">
+        <f t="shared" si="5"/>
+        <v>79.43999999999825</v>
+      </c>
+    </row>
+    <row r="104" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M104" s="12">
+        <v>7.9999999999998996</v>
+      </c>
+      <c r="N104" s="10">
         <f t="shared" si="3"/>
-        <v>7.7999999999999003</v>
-      </c>
-    </row>
-    <row r="104" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M104" s="24">
+        <v>60.999999999999403</v>
+      </c>
+      <c r="O104" s="11">
+        <f t="shared" si="4"/>
         <v>7.9999999999998996</v>
       </c>
-      <c r="N104" s="21">
-        <f t="shared" si="2"/>
-        <v>60.999999999999403</v>
-      </c>
-      <c r="O104" s="23">
+      <c r="P104" s="26">
+        <f t="shared" si="5"/>
+        <v>82.999999999998195</v>
+      </c>
+    </row>
+    <row r="105" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M105" s="12">
+        <v>8.1999999999998998</v>
+      </c>
+      <c r="N105" s="10">
         <f t="shared" si="3"/>
-        <v>7.9999999999998996</v>
-      </c>
-    </row>
-    <row r="105" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M105" s="24">
+        <v>62.199999999999399</v>
+      </c>
+      <c r="O105" s="11">
+        <f t="shared" si="4"/>
         <v>8.1999999999998998</v>
       </c>
-      <c r="N105" s="21">
-        <f t="shared" si="2"/>
-        <v>62.199999999999399</v>
-      </c>
-      <c r="O105" s="23">
+      <c r="P105" s="26">
+        <f t="shared" si="5"/>
+        <v>86.639999999998167</v>
+      </c>
+    </row>
+    <row r="106" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M106" s="12">
+        <v>8.3999999999999009</v>
+      </c>
+      <c r="N106" s="10">
         <f t="shared" si="3"/>
-        <v>8.1999999999998998</v>
-      </c>
-    </row>
-    <row r="106" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M106" s="24">
+        <v>63.399999999999409</v>
+      </c>
+      <c r="O106" s="11">
+        <f t="shared" si="4"/>
         <v>8.3999999999999009</v>
       </c>
-      <c r="N106" s="21">
-        <f t="shared" si="2"/>
-        <v>63.399999999999409</v>
-      </c>
-      <c r="O106" s="23">
+      <c r="P106" s="26">
+        <f t="shared" si="5"/>
+        <v>90.359999999998138</v>
+      </c>
+    </row>
+    <row r="107" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M107" s="12">
+        <v>8.5999999999999002</v>
+      </c>
+      <c r="N107" s="10">
         <f t="shared" si="3"/>
-        <v>8.3999999999999009</v>
-      </c>
-    </row>
-    <row r="107" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M107" s="24">
+        <v>64.599999999999397</v>
+      </c>
+      <c r="O107" s="11">
+        <f t="shared" si="4"/>
         <v>8.5999999999999002</v>
       </c>
-      <c r="N107" s="21">
-        <f t="shared" si="2"/>
-        <v>64.599999999999397</v>
-      </c>
-      <c r="O107" s="23">
+      <c r="P107" s="26">
+        <f t="shared" si="5"/>
+        <v>94.159999999998092</v>
+      </c>
+    </row>
+    <row r="108" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M108" s="12">
+        <v>8.7999999999998995</v>
+      </c>
+      <c r="N108" s="10">
         <f t="shared" si="3"/>
-        <v>8.5999999999999002</v>
-      </c>
-    </row>
-    <row r="108" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M108" s="24">
+        <v>65.7999999999994</v>
+      </c>
+      <c r="O108" s="11">
+        <f t="shared" si="4"/>
         <v>8.7999999999998995</v>
       </c>
-      <c r="N108" s="21">
-        <f t="shared" si="2"/>
-        <v>65.7999999999994</v>
-      </c>
-      <c r="O108" s="23">
+      <c r="P108" s="26">
+        <f t="shared" si="5"/>
+        <v>98.039999999998031</v>
+      </c>
+    </row>
+    <row r="109" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M109" s="12">
+        <v>8.9999999999999005</v>
+      </c>
+      <c r="N109" s="10">
         <f t="shared" si="3"/>
-        <v>8.7999999999998995</v>
-      </c>
-    </row>
-    <row r="109" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M109" s="24">
+        <v>66.999999999999403</v>
+      </c>
+      <c r="O109" s="11">
+        <f t="shared" si="4"/>
         <v>8.9999999999999005</v>
       </c>
-      <c r="N109" s="21">
-        <f t="shared" si="2"/>
-        <v>66.999999999999403</v>
-      </c>
-      <c r="O109" s="23">
+      <c r="P109" s="26">
+        <f t="shared" si="5"/>
+        <v>101.99999999999801</v>
+      </c>
+    </row>
+    <row r="110" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M110" s="12">
+        <v>9.1999999999998998</v>
+      </c>
+      <c r="N110" s="10">
         <f t="shared" si="3"/>
-        <v>8.9999999999999005</v>
-      </c>
-    </row>
-    <row r="110" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M110" s="24">
+        <v>68.199999999999392</v>
+      </c>
+      <c r="O110" s="11">
+        <f t="shared" si="4"/>
         <v>9.1999999999998998</v>
       </c>
-      <c r="N110" s="21">
-        <f t="shared" si="2"/>
-        <v>68.199999999999392</v>
-      </c>
-      <c r="O110" s="23">
+      <c r="P110" s="26">
+        <f t="shared" si="5"/>
+        <v>106.03999999999795</v>
+      </c>
+    </row>
+    <row r="111" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M111" s="12">
+        <v>9.3999999999999009</v>
+      </c>
+      <c r="N111" s="10">
         <f t="shared" si="3"/>
-        <v>9.1999999999998998</v>
-      </c>
-    </row>
-    <row r="111" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M111" s="24">
+        <v>69.399999999999409</v>
+      </c>
+      <c r="O111" s="11">
+        <f t="shared" si="4"/>
         <v>9.3999999999999009</v>
       </c>
-      <c r="N111" s="21">
-        <f t="shared" si="2"/>
-        <v>69.399999999999409</v>
-      </c>
-      <c r="O111" s="23">
+      <c r="P111" s="26">
+        <f t="shared" si="5"/>
+        <v>110.15999999999794</v>
+      </c>
+    </row>
+    <row r="112" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M112" s="12">
+        <v>9.5999999999999002</v>
+      </c>
+      <c r="N112" s="10">
         <f t="shared" si="3"/>
-        <v>9.3999999999999009</v>
-      </c>
-    </row>
-    <row r="112" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M112" s="24">
+        <v>70.599999999999397</v>
+      </c>
+      <c r="O112" s="11">
+        <f t="shared" si="4"/>
         <v>9.5999999999999002</v>
       </c>
-      <c r="N112" s="21">
-        <f t="shared" si="2"/>
-        <v>70.599999999999397</v>
-      </c>
-      <c r="O112" s="23">
+      <c r="P112" s="26">
+        <f t="shared" si="5"/>
+        <v>114.35999999999788</v>
+      </c>
+    </row>
+    <row r="113" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M113" s="12">
+        <v>9.7999999999998995</v>
+      </c>
+      <c r="N113" s="10">
         <f t="shared" si="3"/>
-        <v>9.5999999999999002</v>
-      </c>
-    </row>
-    <row r="113" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M113" s="24">
+        <v>71.7999999999994</v>
+      </c>
+      <c r="O113" s="11">
+        <f t="shared" si="4"/>
         <v>9.7999999999998995</v>
       </c>
-      <c r="N113" s="21">
-        <f t="shared" si="2"/>
-        <v>71.7999999999994</v>
-      </c>
-      <c r="O113" s="23">
+      <c r="P113" s="26">
+        <f t="shared" si="5"/>
+        <v>118.63999999999783</v>
+      </c>
+    </row>
+    <row r="114" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M114" s="12">
+        <v>9.9999999999999005</v>
+      </c>
+      <c r="N114" s="10">
         <f t="shared" si="3"/>
-        <v>9.7999999999998995</v>
-      </c>
-    </row>
-    <row r="114" spans="13:15" x14ac:dyDescent="0.3">
-      <c r="M114" s="24">
+        <v>72.999999999999403</v>
+      </c>
+      <c r="O114" s="11">
+        <f t="shared" si="4"/>
         <v>9.9999999999999005</v>
       </c>
-      <c r="N114" s="21">
-        <f t="shared" si="2"/>
-        <v>72.999999999999403</v>
-      </c>
-      <c r="O114" s="23">
-        <f t="shared" si="3"/>
-        <v>9.9999999999999005</v>
+      <c r="P114" s="26">
+        <f t="shared" si="5"/>
+        <v>122.99999999999781</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="B4:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="N12:N13"/>
     <mergeCell ref="O12:O13"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="B4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajout fonction polynomiale de 3e degré
</commit_message>
<xml_diff>
--- a/EE03.xlsx
+++ b/EE03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olimo\remise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1239C6B0-CF15-4812-88FB-95538D988EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32B12A8-973A-4AB2-8784-F3DF7EB0B319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CC6D29E-86BE-4D22-95F8-090C74A419FC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Fonctions mathématiques</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>P 2e degré</t>
+  </si>
+  <si>
+    <t>P 3e degré</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -326,6 +329,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2317,6 +2326,655 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4311-4F93-9787-68D128188BEB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>p3e</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$M$14:$M$114</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-9.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-8.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-8.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-8.0000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-7.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-7.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-7.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-6.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-6.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-6.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-6.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-6.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-5.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-5.6000000000000201</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-5.4000000000000199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-5.2000000000000197</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-5.0000000000000204</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-4.8000000000000203</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-4.6000000000000201</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-4.4000000000000199</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-4.2000000000000197</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-4.0000000000000204</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.8000000000000198</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-3.6000000000000201</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-3.4000000000000199</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-3.2000000000000202</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-3.00000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-2.80000000000003</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-2.6000000000000298</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-2.4000000000000301</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-2.2000000000000299</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.0000000000000302</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.80000000000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.6000000000000301</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.4000000000000301</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.2000000000000299</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1.00000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.80000000000002902</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.60000000000002995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.400000000000031</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.20000000000002899</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-4.0856207306205799E-14</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.19999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.80000000000000104</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7.3999999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>7.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>7.7999999999999003</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>7.9999999999998996</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>8.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>8.3999999999999009</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>8.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8.7999999999998995</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>8.9999999999999005</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.1999999999998998</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.3999999999999009</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.5999999999999002</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.7999999999998995</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>9.9999999999999005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$Q$14:$Q$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-826</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-774.51200000000017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-725.21599999999989</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-682.06400000000019</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-637.00799999999981</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-594</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-552.99200000000019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-513.93599999999992</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-476.7840000000017</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-441.48800000000165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-408.00000000000176</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-376.27200000000153</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-346.25600000000145</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-317.90400000000136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-291.16800000000131</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-266.00000000000114</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-242.35200000000111</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-220.1760000000011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-199.42400000000106</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-180.04800000000094</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-162.00000000000082</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-145.2320000000008</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-129.6960000000015</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-115.34400000000137</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-102.12800000000124</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-90.00000000000118</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-78.912000000001086</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-68.816000000000969</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-59.664000000000861</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-51.408000000000762</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-44.000000000000711</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-37.392000000000621</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-31.536000000000552</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-26.38400000000048</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-21.888000000000417</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-18.000000000000362</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-14.672000000000461</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-11.856000000000384</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-9.5040000000003211</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-7.5680000000002607</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-6.0000000000002114</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-4.7520000000001659</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-3.7760000000001286</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-3.0240000000000982</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-2.4480000000000754</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-2.0000000000000595</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-1.6320000000000499</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1.2960000000000504</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.94400000000005835</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.52800000000006719</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-1.2256862191861405E-13</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.68799999999999606</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.5840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.7359999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.1920000000000082</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>8.2079999999999984</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>10.863999999999997</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14.016000000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>17.712000000000003</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>26.928000000000004</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>32.543999999999997</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>38.896000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>46.031999999999989</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>62.848000000000013</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>72.623999999999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>83.376000000000005</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>95.151999999999987</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>121.9679999999927</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>137.10399999999211</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>153.45599999999152</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>171.07199999999088</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>189.99999999999017</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>210.28799999998949</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>231.98399999998878</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>255.13599999998806</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>279.7919999999873</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>305.99999999998641</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>333.80799999998561</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>363.26399999998489</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>394.41599999998402</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>427.31199999998319</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>461.99999999998209</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>498.5279999999812</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>536.94399999998029</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>577.29599999997936</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>619.63199999997846</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>663.99999999997715</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>710.44799999997622</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>759.02399999997544</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>809.77599999997415</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>862.7519999999729</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>917.99999999997192</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>975.56799999997054</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1035.5039999999697</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1097.8559999999682</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1162.6719999999668</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1229.9999999999661</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4311-4F93-9787-68D128188BEB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3405,16 +4063,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230CD6A0-05B3-4CAD-B94C-3912BC4D5061}">
-  <dimension ref="A1:P114"/>
+  <dimension ref="A1:Q114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:16" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:17" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +4090,7 @@
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
@@ -3448,7 +4106,7 @@
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
@@ -3472,7 +4130,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
@@ -3496,7 +4154,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="20" t="s">
         <v>3</v>
       </c>
@@ -3516,7 +4174,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
         <v>4</v>
       </c>
@@ -3538,7 +4196,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
@@ -3562,7 +4220,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>6</v>
       </c>
@@ -3588,7 +4246,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>7</v>
       </c>
@@ -3612,7 +4270,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M12" s="13" t="s">
         <v>21</v>
       </c>
@@ -3625,14 +4283,18 @@
       <c r="P12" s="25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q12" s="27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M13" s="13"/>
       <c r="N13" s="14"/>
       <c r="O13" s="15"/>
       <c r="P13" s="25"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q13" s="27"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M14" s="12">
         <v>-10</v>
       </c>
@@ -3648,8 +4310,12 @@
         <f>$F$8*(M14^2)+$G$8*M14+$H$8</f>
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q14" s="28">
+        <f>$F$9*(M14^3)+$G$9*(M14^2)+$H$9*M14+I9</f>
+        <v>-826</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M15" s="12">
         <v>-9.8000000000000007</v>
       </c>
@@ -3665,8 +4331,12 @@
         <f t="shared" ref="P15:P78" si="2">$F$8*(M15^2)+$G$8*M15+$H$8</f>
         <v>79.440000000000026</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q15" s="28">
+        <f t="shared" ref="Q15:Q78" si="3">$F$9*(M15^3)+$G$9*(M15^2)+$H$9*M15+I10</f>
+        <v>-774.51200000000017</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M16" s="12">
         <v>-9.6</v>
       </c>
@@ -3682,8 +4352,12 @@
         <f t="shared" si="2"/>
         <v>75.959999999999994</v>
       </c>
-    </row>
-    <row r="17" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q16" s="28">
+        <f t="shared" si="3"/>
+        <v>-725.21599999999989</v>
+      </c>
+    </row>
+    <row r="17" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M17" s="12">
         <v>-9.4</v>
       </c>
@@ -3699,8 +4373,12 @@
         <f t="shared" si="2"/>
         <v>72.560000000000016</v>
       </c>
-    </row>
-    <row r="18" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q17" s="28">
+        <f t="shared" si="3"/>
+        <v>-682.06400000000019</v>
+      </c>
+    </row>
+    <row r="18" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M18" s="12">
         <v>-9.1999999999999993</v>
       </c>
@@ -3716,8 +4394,12 @@
         <f t="shared" si="2"/>
         <v>69.239999999999981</v>
       </c>
-    </row>
-    <row r="19" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q18" s="28">
+        <f t="shared" si="3"/>
+        <v>-637.00799999999981</v>
+      </c>
+    </row>
+    <row r="19" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M19" s="12">
         <v>-9</v>
       </c>
@@ -3733,8 +4415,12 @@
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q19" s="28">
+        <f t="shared" si="3"/>
+        <v>-594</v>
+      </c>
+    </row>
+    <row r="20" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M20" s="12">
         <v>-8.8000000000000007</v>
       </c>
@@ -3750,8 +4436,12 @@
         <f t="shared" si="2"/>
         <v>62.840000000000011</v>
       </c>
-    </row>
-    <row r="21" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q20" s="28">
+        <f t="shared" si="3"/>
+        <v>-552.99200000000019</v>
+      </c>
+    </row>
+    <row r="21" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M21" s="12">
         <v>-8.6</v>
       </c>
@@ -3767,8 +4457,12 @@
         <f t="shared" si="2"/>
         <v>59.759999999999991</v>
       </c>
-    </row>
-    <row r="22" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q21" s="28">
+        <f t="shared" si="3"/>
+        <v>-513.93599999999992</v>
+      </c>
+    </row>
+    <row r="22" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M22" s="12">
         <v>-8.4000000000000092</v>
       </c>
@@ -3784,8 +4478,12 @@
         <f t="shared" si="2"/>
         <v>56.76000000000014</v>
       </c>
-    </row>
-    <row r="23" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q22" s="28">
+        <f t="shared" si="3"/>
+        <v>-476.7840000000017</v>
+      </c>
+    </row>
+    <row r="23" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M23" s="12">
         <v>-8.2000000000000099</v>
       </c>
@@ -3801,8 +4499,12 @@
         <f t="shared" si="2"/>
         <v>53.840000000000146</v>
       </c>
-    </row>
-    <row r="24" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q23" s="28">
+        <f t="shared" si="3"/>
+        <v>-441.48800000000165</v>
+      </c>
+    </row>
+    <row r="24" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M24" s="12">
         <v>-8.0000000000000107</v>
       </c>
@@ -3818,8 +4520,12 @@
         <f t="shared" si="2"/>
         <v>51.000000000000149</v>
       </c>
-    </row>
-    <row r="25" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q24" s="28">
+        <f t="shared" si="3"/>
+        <v>-408.00000000000176</v>
+      </c>
+    </row>
+    <row r="25" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M25" s="12">
         <v>-7.8000000000000096</v>
       </c>
@@ -3835,8 +4541,12 @@
         <f t="shared" si="2"/>
         <v>48.240000000000137</v>
       </c>
-    </row>
-    <row r="26" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q25" s="28">
+        <f t="shared" si="3"/>
+        <v>-376.27200000000153</v>
+      </c>
+    </row>
+    <row r="26" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M26" s="12">
         <v>-7.6000000000000103</v>
       </c>
@@ -3852,8 +4562,12 @@
         <f t="shared" si="2"/>
         <v>45.56000000000013</v>
       </c>
-    </row>
-    <row r="27" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q26" s="28">
+        <f t="shared" si="3"/>
+        <v>-346.25600000000145</v>
+      </c>
+    </row>
+    <row r="27" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M27" s="12">
         <v>-7.4000000000000101</v>
       </c>
@@ -3869,8 +4583,12 @@
         <f t="shared" si="2"/>
         <v>42.960000000000129</v>
       </c>
-    </row>
-    <row r="28" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q27" s="28">
+        <f t="shared" si="3"/>
+        <v>-317.90400000000136</v>
+      </c>
+    </row>
+    <row r="28" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M28" s="12">
         <v>-7.2000000000000099</v>
       </c>
@@ -3886,8 +4604,12 @@
         <f t="shared" si="2"/>
         <v>40.440000000000126</v>
       </c>
-    </row>
-    <row r="29" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q28" s="28">
+        <f t="shared" si="3"/>
+        <v>-291.16800000000131</v>
+      </c>
+    </row>
+    <row r="29" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M29" s="12">
         <v>-7.0000000000000098</v>
       </c>
@@ -3903,8 +4625,12 @@
         <f t="shared" si="2"/>
         <v>38.000000000000114</v>
       </c>
-    </row>
-    <row r="30" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q29" s="28">
+        <f t="shared" si="3"/>
+        <v>-266.00000000000114</v>
+      </c>
+    </row>
+    <row r="30" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M30" s="12">
         <v>-6.8000000000000096</v>
       </c>
@@ -3920,8 +4646,12 @@
         <f t="shared" si="2"/>
         <v>35.640000000000114</v>
       </c>
-    </row>
-    <row r="31" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q30" s="28">
+        <f t="shared" si="3"/>
+        <v>-242.35200000000111</v>
+      </c>
+    </row>
+    <row r="31" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M31" s="12">
         <v>-6.6000000000000103</v>
       </c>
@@ -3937,8 +4667,12 @@
         <f t="shared" si="2"/>
         <v>33.360000000000113</v>
       </c>
-    </row>
-    <row r="32" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q31" s="28">
+        <f t="shared" si="3"/>
+        <v>-220.1760000000011</v>
+      </c>
+    </row>
+    <row r="32" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M32" s="12">
         <v>-6.4000000000000101</v>
       </c>
@@ -3954,8 +4688,12 @@
         <f t="shared" si="2"/>
         <v>31.16000000000011</v>
       </c>
-    </row>
-    <row r="33" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q32" s="28">
+        <f t="shared" si="3"/>
+        <v>-199.42400000000106</v>
+      </c>
+    </row>
+    <row r="33" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M33" s="12">
         <v>-6.2000000000000099</v>
       </c>
@@ -3971,8 +4709,12 @@
         <f t="shared" si="2"/>
         <v>29.040000000000106</v>
       </c>
-    </row>
-    <row r="34" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q33" s="28">
+        <f t="shared" si="3"/>
+        <v>-180.04800000000094</v>
+      </c>
+    </row>
+    <row r="34" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M34" s="12">
         <v>-6.0000000000000098</v>
       </c>
@@ -3988,8 +4730,12 @@
         <f t="shared" si="2"/>
         <v>27.000000000000092</v>
       </c>
-    </row>
-    <row r="35" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q34" s="28">
+        <f t="shared" si="3"/>
+        <v>-162.00000000000082</v>
+      </c>
+    </row>
+    <row r="35" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M35" s="12">
         <v>-5.8000000000000096</v>
       </c>
@@ -4005,8 +4751,12 @@
         <f t="shared" si="2"/>
         <v>25.040000000000095</v>
       </c>
-    </row>
-    <row r="36" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q35" s="28">
+        <f t="shared" si="3"/>
+        <v>-145.2320000000008</v>
+      </c>
+    </row>
+    <row r="36" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M36" s="12">
         <v>-5.6000000000000201</v>
       </c>
@@ -4022,8 +4772,12 @@
         <f t="shared" si="2"/>
         <v>23.160000000000181</v>
       </c>
-    </row>
-    <row r="37" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q36" s="28">
+        <f t="shared" si="3"/>
+        <v>-129.6960000000015</v>
+      </c>
+    </row>
+    <row r="37" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M37" s="12">
         <v>-5.4000000000000199</v>
       </c>
@@ -4039,8 +4793,12 @@
         <f t="shared" si="2"/>
         <v>21.360000000000174</v>
       </c>
-    </row>
-    <row r="38" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q37" s="28">
+        <f t="shared" si="3"/>
+        <v>-115.34400000000137</v>
+      </c>
+    </row>
+    <row r="38" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M38" s="12">
         <v>-5.2000000000000197</v>
       </c>
@@ -4056,8 +4814,12 @@
         <f t="shared" si="2"/>
         <v>19.640000000000164</v>
       </c>
-    </row>
-    <row r="39" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q38" s="28">
+        <f t="shared" si="3"/>
+        <v>-102.12800000000124</v>
+      </c>
+    </row>
+    <row r="39" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M39" s="12">
         <v>-5.0000000000000204</v>
       </c>
@@ -4073,8 +4835,12 @@
         <f t="shared" si="2"/>
         <v>18.000000000000163</v>
       </c>
-    </row>
-    <row r="40" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q39" s="28">
+        <f t="shared" si="3"/>
+        <v>-90.00000000000118</v>
+      </c>
+    </row>
+    <row r="40" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M40" s="12">
         <v>-4.8000000000000203</v>
       </c>
@@ -4090,8 +4856,12 @@
         <f t="shared" si="2"/>
         <v>16.440000000000154</v>
       </c>
-    </row>
-    <row r="41" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q40" s="28">
+        <f t="shared" si="3"/>
+        <v>-78.912000000001086</v>
+      </c>
+    </row>
+    <row r="41" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M41" s="12">
         <v>-4.6000000000000201</v>
       </c>
@@ -4107,8 +4877,12 @@
         <f t="shared" si="2"/>
         <v>14.960000000000145</v>
       </c>
-    </row>
-    <row r="42" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q41" s="28">
+        <f t="shared" si="3"/>
+        <v>-68.816000000000969</v>
+      </c>
+    </row>
+    <row r="42" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M42" s="12">
         <v>-4.4000000000000199</v>
       </c>
@@ -4124,8 +4898,12 @@
         <f t="shared" si="2"/>
         <v>13.560000000000134</v>
       </c>
-    </row>
-    <row r="43" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q42" s="28">
+        <f t="shared" si="3"/>
+        <v>-59.664000000000861</v>
+      </c>
+    </row>
+    <row r="43" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M43" s="12">
         <v>-4.2000000000000197</v>
       </c>
@@ -4141,8 +4919,12 @@
         <f t="shared" si="2"/>
         <v>12.240000000000125</v>
       </c>
-    </row>
-    <row r="44" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q43" s="28">
+        <f t="shared" si="3"/>
+        <v>-51.408000000000762</v>
+      </c>
+    </row>
+    <row r="44" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M44" s="12">
         <v>-4.0000000000000204</v>
       </c>
@@ -4158,8 +4940,12 @@
         <f t="shared" si="2"/>
         <v>11.000000000000123</v>
       </c>
-    </row>
-    <row r="45" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q44" s="28">
+        <f t="shared" si="3"/>
+        <v>-44.000000000000711</v>
+      </c>
+    </row>
+    <row r="45" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M45" s="12">
         <v>-3.8000000000000198</v>
       </c>
@@ -4175,8 +4961,12 @@
         <f t="shared" si="2"/>
         <v>9.84000000000011</v>
       </c>
-    </row>
-    <row r="46" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q45" s="28">
+        <f t="shared" si="3"/>
+        <v>-37.392000000000621</v>
+      </c>
+    </row>
+    <row r="46" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M46" s="12">
         <v>-3.6000000000000201</v>
       </c>
@@ -4192,8 +4982,12 @@
         <f t="shared" si="2"/>
         <v>8.7600000000001046</v>
       </c>
-    </row>
-    <row r="47" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q46" s="28">
+        <f t="shared" si="3"/>
+        <v>-31.536000000000552</v>
+      </c>
+    </row>
+    <row r="47" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M47" s="12">
         <v>-3.4000000000000199</v>
       </c>
@@ -4209,8 +5003,12 @@
         <f t="shared" si="2"/>
         <v>7.7600000000000957</v>
       </c>
-    </row>
-    <row r="48" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q47" s="28">
+        <f t="shared" si="3"/>
+        <v>-26.38400000000048</v>
+      </c>
+    </row>
+    <row r="48" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M48" s="12">
         <v>-3.2000000000000202</v>
       </c>
@@ -4226,8 +5024,12 @@
         <f t="shared" si="2"/>
         <v>6.8400000000000896</v>
       </c>
-    </row>
-    <row r="49" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q48" s="28">
+        <f t="shared" si="3"/>
+        <v>-21.888000000000417</v>
+      </c>
+    </row>
+    <row r="49" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M49" s="12">
         <v>-3.00000000000002</v>
       </c>
@@ -4243,8 +5045,12 @@
         <f t="shared" si="2"/>
         <v>6.0000000000000808</v>
       </c>
-    </row>
-    <row r="50" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q49" s="28">
+        <f t="shared" si="3"/>
+        <v>-18.000000000000362</v>
+      </c>
+    </row>
+    <row r="50" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M50" s="12">
         <v>-2.80000000000003</v>
       </c>
@@ -4260,8 +5066,12 @@
         <f t="shared" si="2"/>
         <v>5.2400000000001077</v>
       </c>
-    </row>
-    <row r="51" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q50" s="28">
+        <f t="shared" si="3"/>
+        <v>-14.672000000000461</v>
+      </c>
+    </row>
+    <row r="51" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M51" s="12">
         <v>-2.6000000000000298</v>
       </c>
@@ -4277,8 +5087,12 @@
         <f t="shared" si="2"/>
         <v>4.5600000000000955</v>
       </c>
-    </row>
-    <row r="52" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q51" s="28">
+        <f t="shared" si="3"/>
+        <v>-11.856000000000384</v>
+      </c>
+    </row>
+    <row r="52" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M52" s="12">
         <v>-2.4000000000000301</v>
       </c>
@@ -4294,8 +5108,12 @@
         <f t="shared" si="2"/>
         <v>3.9600000000000843</v>
       </c>
-    </row>
-    <row r="53" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q52" s="28">
+        <f t="shared" si="3"/>
+        <v>-9.5040000000003211</v>
+      </c>
+    </row>
+    <row r="53" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M53" s="12">
         <v>-2.2000000000000299</v>
       </c>
@@ -4311,8 +5129,12 @@
         <f t="shared" si="2"/>
         <v>3.4400000000000714</v>
       </c>
-    </row>
-    <row r="54" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q53" s="28">
+        <f t="shared" si="3"/>
+        <v>-7.5680000000002607</v>
+      </c>
+    </row>
+    <row r="54" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M54" s="12">
         <v>-2.0000000000000302</v>
       </c>
@@ -4328,8 +5150,12 @@
         <f t="shared" si="2"/>
         <v>3.0000000000000604</v>
       </c>
-    </row>
-    <row r="55" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q54" s="28">
+        <f t="shared" si="3"/>
+        <v>-6.0000000000002114</v>
+      </c>
+    </row>
+    <row r="55" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M55" s="12">
         <v>-1.80000000000003</v>
       </c>
@@ -4345,8 +5171,12 @@
         <f t="shared" si="2"/>
         <v>2.6400000000000481</v>
       </c>
-    </row>
-    <row r="56" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q55" s="28">
+        <f t="shared" si="3"/>
+        <v>-4.7520000000001659</v>
+      </c>
+    </row>
+    <row r="56" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M56" s="12">
         <v>-1.6000000000000301</v>
       </c>
@@ -4362,8 +5192,12 @@
         <f t="shared" si="2"/>
         <v>2.3600000000000363</v>
       </c>
-    </row>
-    <row r="57" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q56" s="28">
+        <f t="shared" si="3"/>
+        <v>-3.7760000000001286</v>
+      </c>
+    </row>
+    <row r="57" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M57" s="12">
         <v>-1.4000000000000301</v>
       </c>
@@ -4379,8 +5213,12 @@
         <f t="shared" si="2"/>
         <v>2.1600000000000241</v>
       </c>
-    </row>
-    <row r="58" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q57" s="28">
+        <f t="shared" si="3"/>
+        <v>-3.0240000000000982</v>
+      </c>
+    </row>
+    <row r="58" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M58" s="12">
         <v>-1.2000000000000299</v>
       </c>
@@ -4396,8 +5234,12 @@
         <f t="shared" si="2"/>
         <v>2.040000000000012</v>
       </c>
-    </row>
-    <row r="59" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q58" s="28">
+        <f t="shared" si="3"/>
+        <v>-2.4480000000000754</v>
+      </c>
+    </row>
+    <row r="59" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M59" s="12">
         <v>-1.00000000000003</v>
       </c>
@@ -4413,8 +5255,12 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q59" s="28">
+        <f t="shared" si="3"/>
+        <v>-2.0000000000000595</v>
+      </c>
+    </row>
+    <row r="60" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M60" s="12">
         <v>-0.80000000000002902</v>
       </c>
@@ -4430,8 +5276,12 @@
         <f t="shared" si="2"/>
         <v>2.0399999999999885</v>
       </c>
-    </row>
-    <row r="61" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q60" s="28">
+        <f t="shared" si="3"/>
+        <v>-1.6320000000000499</v>
+      </c>
+    </row>
+    <row r="61" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M61" s="12">
         <v>-0.60000000000002995</v>
       </c>
@@ -4447,8 +5297,12 @@
         <f t="shared" si="2"/>
         <v>2.1599999999999762</v>
       </c>
-    </row>
-    <row r="62" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q61" s="28">
+        <f t="shared" si="3"/>
+        <v>-1.2960000000000504</v>
+      </c>
+    </row>
+    <row r="62" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M62" s="12">
         <v>-0.400000000000031</v>
       </c>
@@ -4464,8 +5318,12 @@
         <f t="shared" si="2"/>
         <v>2.359999999999963</v>
       </c>
-    </row>
-    <row r="63" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q62" s="28">
+        <f t="shared" si="3"/>
+        <v>-0.94400000000005835</v>
+      </c>
+    </row>
+    <row r="63" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M63" s="12">
         <v>-0.20000000000002899</v>
       </c>
@@ -4481,8 +5339,12 @@
         <f t="shared" si="2"/>
         <v>2.6399999999999535</v>
       </c>
-    </row>
-    <row r="64" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q63" s="28">
+        <f t="shared" si="3"/>
+        <v>-0.52800000000006719</v>
+      </c>
+    </row>
+    <row r="64" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M64" s="12">
         <v>-4.0856207306205799E-14</v>
       </c>
@@ -4498,8 +5360,12 @@
         <f t="shared" si="2"/>
         <v>2.9999999999999183</v>
       </c>
-    </row>
-    <row r="65" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q64" s="28">
+        <f t="shared" si="3"/>
+        <v>-1.2256862191861405E-13</v>
+      </c>
+    </row>
+    <row r="65" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M65" s="12">
         <v>0.19999999999999901</v>
       </c>
@@ -4515,8 +5381,12 @@
         <f t="shared" si="2"/>
         <v>3.4399999999999977</v>
       </c>
-    </row>
-    <row r="66" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q65" s="28">
+        <f t="shared" si="3"/>
+        <v>0.68799999999999606</v>
+      </c>
+    </row>
+    <row r="66" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M66" s="12">
         <v>0.4</v>
       </c>
@@ -4532,8 +5402,12 @@
         <f t="shared" si="2"/>
         <v>3.96</v>
       </c>
-    </row>
-    <row r="67" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q66" s="28">
+        <f t="shared" si="3"/>
+        <v>1.5840000000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M67" s="12">
         <v>0.6</v>
       </c>
@@ -4549,8 +5423,12 @@
         <f t="shared" si="2"/>
         <v>4.5600000000000005</v>
       </c>
-    </row>
-    <row r="68" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q67" s="28">
+        <f t="shared" si="3"/>
+        <v>2.7359999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M68" s="12">
         <v>0.80000000000000104</v>
       </c>
@@ -4566,8 +5444,12 @@
         <f t="shared" si="2"/>
         <v>5.2400000000000038</v>
       </c>
-    </row>
-    <row r="69" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q68" s="28">
+        <f t="shared" si="3"/>
+        <v>4.1920000000000082</v>
+      </c>
+    </row>
+    <row r="69" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M69" s="12">
         <v>1</v>
       </c>
@@ -4583,8 +5465,12 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q69" s="28">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M70" s="12">
         <v>1.2</v>
       </c>
@@ -4600,8 +5486,12 @@
         <f t="shared" si="2"/>
         <v>6.84</v>
       </c>
-    </row>
-    <row r="71" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q70" s="28">
+        <f t="shared" si="3"/>
+        <v>8.2079999999999984</v>
+      </c>
+    </row>
+    <row r="71" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M71" s="12">
         <v>1.4</v>
       </c>
@@ -4617,8 +5507,12 @@
         <f t="shared" si="2"/>
         <v>7.76</v>
       </c>
-    </row>
-    <row r="72" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q71" s="28">
+        <f t="shared" si="3"/>
+        <v>10.863999999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M72" s="12">
         <v>1.6</v>
       </c>
@@ -4634,8 +5528,12 @@
         <f t="shared" si="2"/>
         <v>8.7600000000000016</v>
       </c>
-    </row>
-    <row r="73" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q72" s="28">
+        <f t="shared" si="3"/>
+        <v>14.016000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M73" s="12">
         <v>1.8</v>
       </c>
@@ -4651,8 +5549,12 @@
         <f t="shared" si="2"/>
         <v>9.84</v>
       </c>
-    </row>
-    <row r="74" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q73" s="28">
+        <f t="shared" si="3"/>
+        <v>17.712000000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M74" s="12">
         <v>2</v>
       </c>
@@ -4668,8 +5570,12 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="75" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q74" s="28">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M75" s="12">
         <v>2.2000000000000002</v>
       </c>
@@ -4685,8 +5591,12 @@
         <f t="shared" si="2"/>
         <v>12.240000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q75" s="28">
+        <f t="shared" si="3"/>
+        <v>26.928000000000004</v>
+      </c>
+    </row>
+    <row r="76" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M76" s="12">
         <v>2.4</v>
       </c>
@@ -4702,8 +5612,12 @@
         <f t="shared" si="2"/>
         <v>13.559999999999999</v>
       </c>
-    </row>
-    <row r="77" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q76" s="28">
+        <f t="shared" si="3"/>
+        <v>32.543999999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M77" s="12">
         <v>2.6</v>
       </c>
@@ -4719,8 +5633,12 @@
         <f t="shared" si="2"/>
         <v>14.96</v>
       </c>
-    </row>
-    <row r="78" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q77" s="28">
+        <f t="shared" si="3"/>
+        <v>38.896000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M78" s="12">
         <v>2.8</v>
       </c>
@@ -4736,622 +5654,771 @@
         <f t="shared" si="2"/>
         <v>16.439999999999998</v>
       </c>
-    </row>
-    <row r="79" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q78" s="28">
+        <f t="shared" si="3"/>
+        <v>46.031999999999989</v>
+      </c>
+    </row>
+    <row r="79" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M79" s="12">
         <v>3</v>
       </c>
       <c r="N79" s="10">
-        <f t="shared" ref="N79:N114" si="3">$F$6*ABS($G$6*M79+$H$6)+$I$6</f>
+        <f t="shared" ref="N79:N114" si="4">$F$6*ABS($G$6*M79+$H$6)+$I$6</f>
         <v>31</v>
       </c>
       <c r="O79" s="11">
-        <f t="shared" ref="O79:O114" si="4">$F$7*M79+G72</f>
+        <f t="shared" ref="O79:O114" si="5">$F$7*M79+G72</f>
         <v>3</v>
       </c>
       <c r="P79" s="26">
-        <f t="shared" ref="P79:P114" si="5">$F$8*(M79^2)+$G$8*M79+$H$8</f>
+        <f t="shared" ref="P79:P114" si="6">$F$8*(M79^2)+$G$8*M79+$H$8</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="80" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q79" s="28">
+        <f t="shared" ref="Q79:Q114" si="7">$F$9*(M79^3)+$G$9*(M79^2)+$H$9*M79+I74</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M80" s="12">
         <v>3.2</v>
       </c>
       <c r="N80" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32.200000000000003</v>
       </c>
       <c r="O80" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2</v>
       </c>
       <c r="P80" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19.64</v>
       </c>
-    </row>
-    <row r="81" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q80" s="28">
+        <f t="shared" si="7"/>
+        <v>62.848000000000013</v>
+      </c>
+    </row>
+    <row r="81" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M81" s="12">
         <v>3.4</v>
       </c>
       <c r="N81" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.400000000000006</v>
       </c>
       <c r="O81" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.4</v>
       </c>
       <c r="P81" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21.36</v>
       </c>
-    </row>
-    <row r="82" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q81" s="28">
+        <f t="shared" si="7"/>
+        <v>72.623999999999995</v>
+      </c>
+    </row>
+    <row r="82" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M82" s="12">
         <v>3.6</v>
       </c>
       <c r="N82" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>34.599999999999994</v>
       </c>
       <c r="O82" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6</v>
       </c>
       <c r="P82" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23.16</v>
       </c>
-    </row>
-    <row r="83" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q82" s="28">
+        <f t="shared" si="7"/>
+        <v>83.376000000000005</v>
+      </c>
+    </row>
+    <row r="83" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M83" s="12">
         <v>3.8</v>
       </c>
       <c r="N83" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35.799999999999997</v>
       </c>
       <c r="O83" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8</v>
       </c>
       <c r="P83" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25.04</v>
       </c>
-    </row>
-    <row r="84" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q83" s="28">
+        <f t="shared" si="7"/>
+        <v>95.151999999999987</v>
+      </c>
+    </row>
+    <row r="84" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M84" s="12">
         <v>4</v>
       </c>
       <c r="N84" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37</v>
       </c>
       <c r="O84" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P84" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="85" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q84" s="28">
+        <f t="shared" si="7"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M85" s="12">
         <v>4.1999999999998998</v>
       </c>
       <c r="N85" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38.199999999999399</v>
       </c>
       <c r="O85" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.1999999999998998</v>
       </c>
       <c r="P85" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29.039999999998958</v>
       </c>
-    </row>
-    <row r="86" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q85" s="28">
+        <f t="shared" si="7"/>
+        <v>121.9679999999927</v>
+      </c>
+    </row>
+    <row r="86" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M86" s="12">
         <v>4.3999999999999</v>
       </c>
       <c r="N86" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.399999999999402</v>
       </c>
       <c r="O86" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.3999999999999</v>
       </c>
       <c r="P86" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31.159999999998917</v>
       </c>
-    </row>
-    <row r="87" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q86" s="28">
+        <f t="shared" si="7"/>
+        <v>137.10399999999211</v>
+      </c>
+    </row>
+    <row r="87" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M87" s="12">
         <v>4.5999999999999002</v>
       </c>
       <c r="N87" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40.599999999999397</v>
       </c>
       <c r="O87" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5999999999999002</v>
       </c>
       <c r="P87" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33.359999999998877</v>
       </c>
-    </row>
-    <row r="88" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q87" s="28">
+        <f t="shared" si="7"/>
+        <v>153.45599999999152</v>
+      </c>
+    </row>
+    <row r="88" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M88" s="12">
         <v>4.7999999999999003</v>
       </c>
       <c r="N88" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>41.7999999999994</v>
       </c>
       <c r="O88" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.7999999999999003</v>
       </c>
       <c r="P88" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35.639999999998842</v>
       </c>
-    </row>
-    <row r="89" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q88" s="28">
+        <f t="shared" si="7"/>
+        <v>171.07199999999088</v>
+      </c>
+    </row>
+    <row r="89" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M89" s="12">
         <v>4.9999999999998996</v>
       </c>
       <c r="N89" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>42.999999999999396</v>
       </c>
       <c r="O89" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.9999999999998996</v>
       </c>
       <c r="P89" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37.999999999998799</v>
       </c>
-    </row>
-    <row r="90" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q89" s="28">
+        <f t="shared" si="7"/>
+        <v>189.99999999999017</v>
+      </c>
+    </row>
+    <row r="90" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M90" s="12">
         <v>5.1999999999998998</v>
       </c>
       <c r="N90" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44.199999999999399</v>
       </c>
       <c r="O90" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.1999999999998998</v>
       </c>
       <c r="P90" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40.439999999998761</v>
       </c>
-    </row>
-    <row r="91" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q90" s="28">
+        <f t="shared" si="7"/>
+        <v>210.28799999998949</v>
+      </c>
+    </row>
+    <row r="91" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M91" s="12">
         <v>5.3999999999999</v>
       </c>
       <c r="N91" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45.399999999999402</v>
       </c>
       <c r="O91" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.3999999999999</v>
       </c>
       <c r="P91" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42.959999999998722</v>
       </c>
-    </row>
-    <row r="92" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q91" s="28">
+        <f t="shared" si="7"/>
+        <v>231.98399999998878</v>
+      </c>
+    </row>
+    <row r="92" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M92" s="12">
         <v>5.5999999999999002</v>
       </c>
       <c r="N92" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46.599999999999397</v>
       </c>
       <c r="O92" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.5999999999999002</v>
       </c>
       <c r="P92" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45.559999999998681</v>
       </c>
-    </row>
-    <row r="93" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q92" s="28">
+        <f t="shared" si="7"/>
+        <v>255.13599999998806</v>
+      </c>
+    </row>
+    <row r="93" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M93" s="12">
         <v>5.7999999999999003</v>
       </c>
       <c r="N93" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47.7999999999994</v>
       </c>
       <c r="O93" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.7999999999999003</v>
       </c>
       <c r="P93" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>48.239999999998645</v>
       </c>
-    </row>
-    <row r="94" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q93" s="28">
+        <f t="shared" si="7"/>
+        <v>279.7919999999873</v>
+      </c>
+    </row>
+    <row r="94" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M94" s="12">
         <v>5.9999999999998996</v>
       </c>
       <c r="N94" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48.999999999999396</v>
       </c>
       <c r="O94" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.9999999999998996</v>
       </c>
       <c r="P94" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50.999999999998593</v>
       </c>
-    </row>
-    <row r="95" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q94" s="28">
+        <f t="shared" si="7"/>
+        <v>305.99999999998641</v>
+      </c>
+    </row>
+    <row r="95" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M95" s="12">
         <v>6.1999999999998998</v>
       </c>
       <c r="N95" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50.199999999999399</v>
       </c>
       <c r="O95" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.1999999999998998</v>
       </c>
       <c r="P95" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53.839999999998554</v>
       </c>
-    </row>
-    <row r="96" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q95" s="28">
+        <f t="shared" si="7"/>
+        <v>333.80799999998561</v>
+      </c>
+    </row>
+    <row r="96" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M96" s="12">
         <v>6.3999999999999</v>
       </c>
       <c r="N96" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51.399999999999402</v>
       </c>
       <c r="O96" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.3999999999999</v>
       </c>
       <c r="P96" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56.75999999999852</v>
       </c>
-    </row>
-    <row r="97" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q96" s="28">
+        <f t="shared" si="7"/>
+        <v>363.26399999998489</v>
+      </c>
+    </row>
+    <row r="97" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M97" s="12">
         <v>6.5999999999999002</v>
       </c>
       <c r="N97" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52.599999999999397</v>
       </c>
       <c r="O97" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.5999999999999002</v>
       </c>
       <c r="P97" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59.759999999998485</v>
       </c>
-    </row>
-    <row r="98" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q97" s="28">
+        <f t="shared" si="7"/>
+        <v>394.41599999998402</v>
+      </c>
+    </row>
+    <row r="98" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M98" s="12">
         <v>6.7999999999999003</v>
       </c>
       <c r="N98" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53.799999999999407</v>
       </c>
       <c r="O98" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.7999999999999003</v>
       </c>
       <c r="P98" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.839999999998447</v>
       </c>
-    </row>
-    <row r="99" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q98" s="28">
+        <f t="shared" si="7"/>
+        <v>427.31199999998319</v>
+      </c>
+    </row>
+    <row r="99" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M99" s="12">
         <v>6.9999999999998996</v>
       </c>
       <c r="N99" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54.999999999999403</v>
       </c>
       <c r="O99" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.9999999999998996</v>
       </c>
       <c r="P99" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>65.999999999998394</v>
       </c>
-    </row>
-    <row r="100" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q99" s="28">
+        <f t="shared" si="7"/>
+        <v>461.99999999998209</v>
+      </c>
+    </row>
+    <row r="100" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M100" s="12">
         <v>7.1999999999998998</v>
       </c>
       <c r="N100" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56.199999999999399</v>
       </c>
       <c r="O100" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.1999999999998998</v>
       </c>
       <c r="P100" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69.239999999998361</v>
       </c>
-    </row>
-    <row r="101" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q100" s="28">
+        <f t="shared" si="7"/>
+        <v>498.5279999999812</v>
+      </c>
+    </row>
+    <row r="101" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M101" s="12">
         <v>7.3999999999999</v>
       </c>
       <c r="N101" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57.399999999999395</v>
       </c>
       <c r="O101" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.3999999999999</v>
       </c>
       <c r="P101" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72.559999999998325</v>
       </c>
-    </row>
-    <row r="102" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q101" s="28">
+        <f t="shared" si="7"/>
+        <v>536.94399999998029</v>
+      </c>
+    </row>
+    <row r="102" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M102" s="12">
         <v>7.5999999999999002</v>
       </c>
       <c r="N102" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58.599999999999397</v>
       </c>
       <c r="O102" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.5999999999999002</v>
       </c>
       <c r="P102" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75.959999999998288</v>
       </c>
-    </row>
-    <row r="103" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q102" s="28">
+        <f t="shared" si="7"/>
+        <v>577.29599999997936</v>
+      </c>
+    </row>
+    <row r="103" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M103" s="12">
         <v>7.7999999999999003</v>
       </c>
       <c r="N103" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59.799999999999407</v>
       </c>
       <c r="O103" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.7999999999999003</v>
       </c>
       <c r="P103" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79.43999999999825</v>
       </c>
-    </row>
-    <row r="104" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q103" s="28">
+        <f t="shared" si="7"/>
+        <v>619.63199999997846</v>
+      </c>
+    </row>
+    <row r="104" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M104" s="12">
         <v>7.9999999999998996</v>
       </c>
       <c r="N104" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60.999999999999403</v>
       </c>
       <c r="O104" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.9999999999998996</v>
       </c>
       <c r="P104" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>82.999999999998195</v>
       </c>
-    </row>
-    <row r="105" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q104" s="28">
+        <f t="shared" si="7"/>
+        <v>663.99999999997715</v>
+      </c>
+    </row>
+    <row r="105" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M105" s="12">
         <v>8.1999999999998998</v>
       </c>
       <c r="N105" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62.199999999999399</v>
       </c>
       <c r="O105" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.1999999999998998</v>
       </c>
       <c r="P105" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>86.639999999998167</v>
       </c>
-    </row>
-    <row r="106" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q105" s="28">
+        <f t="shared" si="7"/>
+        <v>710.44799999997622</v>
+      </c>
+    </row>
+    <row r="106" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M106" s="12">
         <v>8.3999999999999009</v>
       </c>
       <c r="N106" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>63.399999999999409</v>
       </c>
       <c r="O106" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3999999999999009</v>
       </c>
       <c r="P106" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>90.359999999998138</v>
       </c>
-    </row>
-    <row r="107" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q106" s="28">
+        <f t="shared" si="7"/>
+        <v>759.02399999997544</v>
+      </c>
+    </row>
+    <row r="107" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M107" s="12">
         <v>8.5999999999999002</v>
       </c>
       <c r="N107" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64.599999999999397</v>
       </c>
       <c r="O107" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.5999999999999002</v>
       </c>
       <c r="P107" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>94.159999999998092</v>
       </c>
-    </row>
-    <row r="108" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q107" s="28">
+        <f t="shared" si="7"/>
+        <v>809.77599999997415</v>
+      </c>
+    </row>
+    <row r="108" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M108" s="12">
         <v>8.7999999999998995</v>
       </c>
       <c r="N108" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65.7999999999994</v>
       </c>
       <c r="O108" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.7999999999998995</v>
       </c>
       <c r="P108" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>98.039999999998031</v>
       </c>
-    </row>
-    <row r="109" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q108" s="28">
+        <f t="shared" si="7"/>
+        <v>862.7519999999729</v>
+      </c>
+    </row>
+    <row r="109" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M109" s="12">
         <v>8.9999999999999005</v>
       </c>
       <c r="N109" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.999999999999403</v>
       </c>
       <c r="O109" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.9999999999999005</v>
       </c>
       <c r="P109" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>101.99999999999801</v>
       </c>
-    </row>
-    <row r="110" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q109" s="28">
+        <f t="shared" si="7"/>
+        <v>917.99999999997192</v>
+      </c>
+    </row>
+    <row r="110" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M110" s="12">
         <v>9.1999999999998998</v>
       </c>
       <c r="N110" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.199999999999392</v>
       </c>
       <c r="O110" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1999999999998998</v>
       </c>
       <c r="P110" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>106.03999999999795</v>
       </c>
-    </row>
-    <row r="111" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q110" s="28">
+        <f t="shared" si="7"/>
+        <v>975.56799999997054</v>
+      </c>
+    </row>
+    <row r="111" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M111" s="12">
         <v>9.3999999999999009</v>
       </c>
       <c r="N111" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69.399999999999409</v>
       </c>
       <c r="O111" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.3999999999999009</v>
       </c>
       <c r="P111" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110.15999999999794</v>
       </c>
-    </row>
-    <row r="112" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q111" s="28">
+        <f t="shared" si="7"/>
+        <v>1035.5039999999697</v>
+      </c>
+    </row>
+    <row r="112" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M112" s="12">
         <v>9.5999999999999002</v>
       </c>
       <c r="N112" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70.599999999999397</v>
       </c>
       <c r="O112" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.5999999999999002</v>
       </c>
       <c r="P112" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>114.35999999999788</v>
       </c>
-    </row>
-    <row r="113" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q112" s="28">
+        <f t="shared" si="7"/>
+        <v>1097.8559999999682</v>
+      </c>
+    </row>
+    <row r="113" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M113" s="12">
         <v>9.7999999999998995</v>
       </c>
       <c r="N113" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71.7999999999994</v>
       </c>
       <c r="O113" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.7999999999998995</v>
       </c>
       <c r="P113" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>118.63999999999783</v>
       </c>
-    </row>
-    <row r="114" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="Q113" s="28">
+        <f t="shared" si="7"/>
+        <v>1162.6719999999668</v>
+      </c>
+    </row>
+    <row r="114" spans="13:17" x14ac:dyDescent="0.3">
       <c r="M114" s="12">
         <v>9.9999999999999005</v>
       </c>
       <c r="N114" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72.999999999999403</v>
       </c>
       <c r="O114" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.9999999999999005</v>
       </c>
       <c r="P114" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>122.99999999999781</v>
       </c>
+      <c r="Q114" s="28">
+        <f t="shared" si="7"/>
+        <v>1229.9999999999661</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
     <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>

</xml_diff>